<commit_message>
AR: cap 3 e 4, 2° modifica.
modifica xlsx requisiti e creazione xlsx tracciamento
</commit_message>
<xml_diff>
--- a/RP/Esterni/Analisi dei Requisiti/Requisiti.xlsx
+++ b/RP/Esterni/Analisi dei Requisiti/Requisiti.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="272">
   <si>
     <t>Codice</t>
   </si>
@@ -89,9 +89,6 @@
     <t>Le funzioni del sistema offerte al \uline{Dipendente} dovranno essere fruibili tramite interfaccia \uline{web}</t>
   </si>
   <si>
-    <t>Dinamica</t>
-  </si>
-  <si>
     <t>Test / Dinamica</t>
   </si>
   <si>
@@ -110,9 +107,6 @@
     <t>Sarà fornita documentazione esaustiva di tutte le classi chiave ed interfacce del prodotto</t>
   </si>
   <si>
-    <t>Sarà fornito un manuale ad uso \uline{Amministratore Sicurezza} riguardo le azioni che potrà compiere tale \uline{Utente}</t>
-  </si>
-  <si>
     <t>Le interfacce che saranno visibili ai \uline{Dipendenti} dovranno essere accattivanti e le funzionalità quanto più intuitive, così da invogliare l'utilizzo</t>
   </si>
   <si>
@@ -179,15 +173,6 @@
     <t>UCAA 1.2</t>
   </si>
   <si>
-    <t>UCAS 2.1</t>
-  </si>
-  <si>
-    <t>UCAS 2.2</t>
-  </si>
-  <si>
-    <t>UCAS 2.3</t>
-  </si>
-  <si>
     <t>UCD 1.1</t>
   </si>
   <si>
@@ -230,9 +215,6 @@
     <t>Le informazioni che un \uline{Dipendente} potrà consultare  sono: storico delle risposte(sia corrette che errate), classifica aziendale, trofei/badge raccolti, statistiche derivanti dalle risposte</t>
   </si>
   <si>
-    <t>Un \uline{Amministratore Azienda} avrà la possibiltà di modificare i dati personali dei Dipendenti</t>
-  </si>
-  <si>
     <t>I campi che potranno essere modificati sono: nome, cognome, indirizzo email, impiego, codice fiscale</t>
   </si>
   <si>
@@ -251,9 +233,6 @@
     <t>Un \uline{Amministratore Sicurezza} che vuole inserire una nuova domanda dovrà specificarne l'eventuale tempo limite di risposta</t>
   </si>
   <si>
-    <t>Un \uline{Amministratore Sicurezza} che vuole inserire una nuova domanda dovrà specificarne la categoria di \uline{Utenti} a cui potrà essere visualizzata</t>
-  </si>
-  <si>
     <t>Un \uline{Amministratore Sicurezza} che vuole inserire una nuova domanda dovrà specificarne l'eventuale percorso di immagine/video di supporto</t>
   </si>
   <si>
@@ -284,9 +263,6 @@
     <t>Un \uline{Amministratore Sicurezza} avrà la possibilità di consultare il tipo di ogni piattaforma sulla quale può essere proposta ogni domanda dell'azienda</t>
   </si>
   <si>
-    <t>Un \uline{Amministratore Sicurezza} avrà la possibilità di consultare la categoria di utenti a cui verrà somministrata ogni domanda dell'azienda</t>
-  </si>
-  <si>
     <t>Un \uline{Amministratore Sicurezza} avrà la possibilità di consultare le immagini/video di ogni domanda dell'azienda</t>
   </si>
   <si>
@@ -431,18 +407,9 @@
     <t>Un \uline{Utente} che ha smarrito la propria password per accedere al sistema potrà recuperarla</t>
   </si>
   <si>
-    <t>Un \uline{Utente} che ha smarrito la password ed ha eseguito la procedura di recupero e non ha ancora effettuato il primo login, la riceverà sulla propria casella di posta elettronica</t>
-  </si>
-  <si>
-    <t>Un \uline{Utente} che ha smarrito la password ed ha eseguito la procedura di recupero ed ha avuto accesso al sistema almeno una volta, riceverà una mail contenente una nuova password ottenuta in modo randomico</t>
-  </si>
-  <si>
     <t>Il sistema permetterà agli \uline{Utenti Autenticati} di effettuare il logout, ma non di terminare l'applicazione</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>UCAA 1.1</t>
   </si>
   <si>
@@ -470,24 +437,6 @@
     <t>UTENTE</t>
   </si>
   <si>
-    <t>Il modulo di registrazione richiederà i dati personali del dipendente</t>
-  </si>
-  <si>
-    <t>Il modulo di registrazione richiederà il nome del dipendente</t>
-  </si>
-  <si>
-    <t>Il modulo di registrazione richiederà il cognome del dipendente</t>
-  </si>
-  <si>
-    <t>Il modulo di registrazione richiederà il codice fiscale del dipendente</t>
-  </si>
-  <si>
-    <t>Il modulo di registrazione richiederà l'indirizzo email del dipendente</t>
-  </si>
-  <si>
-    <t>Il modulo di registrazione richiederà l'impiego del dipendente</t>
-  </si>
-  <si>
     <t>GENERALI</t>
   </si>
   <si>
@@ -503,9 +452,6 @@
     <t>AMMINISTRATORE INSTALLATORE</t>
   </si>
   <si>
-    <t>ROD 8.2</t>
-  </si>
-  <si>
     <t>RPOB 1</t>
   </si>
   <si>
@@ -596,9 +542,6 @@
     <t>RFOB 3.1</t>
   </si>
   <si>
-    <t>RFOB 3.2</t>
-  </si>
-  <si>
     <t>RFOB 4</t>
   </si>
   <si>
@@ -843,14 +786,70 @@
   </si>
   <si>
     <t>RFOB 27.3</t>
+  </si>
+  <si>
+    <t>RFD 8.2</t>
+  </si>
+  <si>
+    <t>Il modulo di registrazione richiederà i dati personali del \uline{Dipendente}</t>
+  </si>
+  <si>
+    <t>Il modulo di registrazione richiederà il nome del \uline{Dipendente}</t>
+  </si>
+  <si>
+    <t>Il modulo di registrazione richiederà il cognome del \uline{Dipendente}</t>
+  </si>
+  <si>
+    <t>Il modulo di registrazione richiederà il codice fiscale del \uline{Dipendente}</t>
+  </si>
+  <si>
+    <t>Il modulo di registrazione richiederà l'indirizzo email del \uline{Dipendente}</t>
+  </si>
+  <si>
+    <t>Il modulo di registrazione richiederà l'impiego del \uline{Dipendente}</t>
+  </si>
+  <si>
+    <t>Un \uline{Amministratore Azienda} avrà la possibiltà di modificare i dati personali dei \uline{Dipendenti}</t>
+  </si>
+  <si>
+    <t>Un \uline{Amministratore Sicurezza} avrà la possibilità di consultare la categoria di \uline{Dipendenti} a cui verrà somministrata ogni domanda dell'azienda</t>
+  </si>
+  <si>
+    <t>Un \uline{Amministratore Sicurezza} che vuole inserire una nuova domanda dovrà specificarne la categoria di \uline{Dipendenti} a cui potrà essere visualizzata</t>
+  </si>
+  <si>
+    <t>UCASA 2.1</t>
+  </si>
+  <si>
+    <t>UCASA 2.3</t>
+  </si>
+  <si>
+    <t>UCASA 2.2</t>
+  </si>
+  <si>
+    <t>Sarà fornito un manuale ad uso \uline{Amministratore Sicurezza} riguardo le azioni che potrà compiere</t>
+  </si>
+  <si>
+    <t>Un \uline{Utente} che ha smarrito la password ed ha eseguito la procedura di recupero, la riceverà sulla propria casella di posta elettronica</t>
+  </si>
+  <si>
+    <t>Statica</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -878,12 +877,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1183,10 +1185,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D100"/>
+  <dimension ref="A1:D126"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D100"/>
+    <sheetView topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1198,55 +1200,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="A1" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="A5" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>189</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>107</v>
+        <v>171</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
@@ -1257,74 +1259,74 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>137</v>
+        <v>270</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>193</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
+    <row r="11" spans="1:4">
+      <c r="A11" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="A12" t="s">
+        <v>175</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C13" t="s">
         <v>13</v>
@@ -1335,10 +1337,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
@@ -1349,10 +1351,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C15" t="s">
         <v>13</v>
@@ -1361,12 +1363,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" ht="30">
       <c r="A16" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
@@ -1375,12 +1377,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C17" t="s">
         <v>13</v>
@@ -1391,13 +1393,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>199</v>
+        <v>256</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="D18" t="s">
         <v>12</v>
@@ -1405,13 +1407,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="D19" t="s">
         <v>12</v>
@@ -1419,10 +1421,10 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>200</v>
+        <v>182</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C20" t="s">
         <v>14</v>
@@ -1433,10 +1435,10 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C21" t="s">
         <v>14</v>
@@ -1447,10 +1449,10 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C22" t="s">
         <v>14</v>
@@ -1461,10 +1463,10 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>203</v>
+        <v>185</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C23" t="s">
         <v>14</v>
@@ -1475,10 +1477,10 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>204</v>
+        <v>186</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C24" t="s">
         <v>14</v>
@@ -1489,13 +1491,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C25" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="D25" t="s">
         <v>12</v>
@@ -1503,13 +1505,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>206</v>
+        <v>188</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
@@ -1517,13 +1519,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="C27" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D27" t="s">
         <v>12</v>
@@ -1531,13 +1533,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C28" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D28" t="s">
         <v>12</v>
@@ -1545,13 +1547,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C29" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D29" t="s">
         <v>12</v>
@@ -1559,13 +1561,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C30" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D30" t="s">
         <v>12</v>
@@ -1573,13 +1575,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C31" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
@@ -1587,111 +1589,111 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C32" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D32" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" ht="30">
       <c r="A33" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>142</v>
+        <v>60</v>
       </c>
       <c r="C33" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="D33" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C34" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D34" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="30">
       <c r="A35" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C35" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D35" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="30">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C36" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D36" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="30">
       <c r="A37" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C37" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D37" t="s">
-        <v>12</v>
+        <v>271</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="30">
       <c r="A38" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>69</v>
+        <v>105</v>
       </c>
       <c r="C38" t="s">
-        <v>57</v>
+        <v>130</v>
       </c>
       <c r="D38" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C39" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="D39" t="s">
         <v>12</v>
@@ -1699,147 +1701,147 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C40" t="s">
+        <v>130</v>
+      </c>
+      <c r="D40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="D40" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" t="s">
-        <v>221</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C41" t="s">
-        <v>141</v>
-      </c>
-      <c r="D41" t="s">
-        <v>12</v>
-      </c>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
+      <c r="A43" t="s">
+        <v>203</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C43" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>112</v>
+        <v>257</v>
       </c>
       <c r="C44" t="s">
         <v>14</v>
       </c>
       <c r="D44" t="s">
-        <v>12</v>
+        <v>271</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>150</v>
+        <v>258</v>
       </c>
       <c r="C45" t="s">
         <v>14</v>
       </c>
       <c r="D45" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>151</v>
+        <v>259</v>
       </c>
       <c r="C46" t="s">
         <v>14</v>
       </c>
       <c r="D46" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>152</v>
+        <v>260</v>
       </c>
       <c r="C47" t="s">
         <v>14</v>
       </c>
       <c r="D47" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>153</v>
+        <v>261</v>
       </c>
       <c r="C48" t="s">
         <v>14</v>
       </c>
       <c r="D48" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>154</v>
+        <v>262</v>
       </c>
       <c r="C49" t="s">
         <v>14</v>
       </c>
       <c r="D49" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>155</v>
+        <v>108</v>
       </c>
       <c r="C50" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="D50" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C51" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D51" t="s">
         <v>12</v>
@@ -1847,13 +1849,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C52" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D52" t="s">
         <v>12</v>
@@ -1861,13 +1863,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C53" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D53" t="s">
         <v>12</v>
@@ -1875,13 +1877,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C54" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D54" t="s">
         <v>12</v>
@@ -1889,13 +1891,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C55" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D55" t="s">
         <v>12</v>
@@ -1903,13 +1905,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C56" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D56" t="s">
         <v>12</v>
@@ -1917,13 +1919,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>122</v>
+        <v>263</v>
       </c>
       <c r="C57" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D57" t="s">
         <v>12</v>
@@ -1931,13 +1933,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>236</v>
+        <v>218</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C58" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D58" t="s">
         <v>12</v>
@@ -1945,49 +1947,49 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>237</v>
+        <v>219</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C59" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D59" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
-      <c r="A60" t="s">
-        <v>238</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C60" t="s">
-        <v>52</v>
-      </c>
-      <c r="D60" t="s">
-        <v>12</v>
-      </c>
+    <row r="61" spans="1:4">
+      <c r="A61" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
+      <c r="A62" t="s">
+        <v>220</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C62" t="s">
+        <v>133</v>
+      </c>
+      <c r="D62" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C63" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="D63" t="s">
         <v>12</v>
@@ -1995,13 +1997,13 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C64" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="D64" t="s">
         <v>12</v>
@@ -2009,13 +2011,13 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C65" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="D65" t="s">
         <v>12</v>
@@ -2023,13 +2025,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C66" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="D66" t="s">
         <v>12</v>
@@ -2037,55 +2039,55 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C67" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="D67" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" ht="30">
       <c r="A68" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>89</v>
+        <v>264</v>
       </c>
       <c r="C68" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="D68" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" ht="30">
       <c r="A69" t="s">
-        <v>245</v>
+        <v>227</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C69" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="D69" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="30">
+    <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C70" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="D70" t="s">
         <v>12</v>
@@ -2093,13 +2095,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C71" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="D71" t="s">
         <v>12</v>
@@ -2107,13 +2109,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C72" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="D72" t="s">
         <v>12</v>
@@ -2121,13 +2123,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>249</v>
+        <v>231</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C73" t="s">
-        <v>145</v>
+        <v>266</v>
       </c>
       <c r="D73" t="s">
         <v>12</v>
@@ -2135,153 +2137,153 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C74" t="s">
-        <v>53</v>
+        <v>266</v>
       </c>
       <c r="D74" t="s">
-        <v>12</v>
+        <v>271</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C75" t="s">
-        <v>53</v>
+        <v>266</v>
       </c>
       <c r="D75" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C76" t="s">
-        <v>53</v>
+        <v>266</v>
       </c>
       <c r="D76" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C77" t="s">
-        <v>53</v>
+        <v>266</v>
       </c>
       <c r="D77" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C78" t="s">
-        <v>53</v>
+        <v>266</v>
       </c>
       <c r="D78" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="30">
       <c r="A79" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>78</v>
+        <v>265</v>
       </c>
       <c r="C79" t="s">
-        <v>53</v>
+        <v>266</v>
       </c>
       <c r="D79" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="30">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C80" t="s">
-        <v>53</v>
+        <v>266</v>
       </c>
       <c r="D80" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C81" t="s">
-        <v>53</v>
+        <v>266</v>
       </c>
       <c r="D81" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C82" t="s">
-        <v>53</v>
+        <v>268</v>
       </c>
       <c r="D82" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="30">
       <c r="A83" t="s">
-        <v>259</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>74</v>
+        <v>241</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="C83" t="s">
-        <v>54</v>
+        <v>268</v>
       </c>
       <c r="D83" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="30">
+    <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>260</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>63</v>
+        <v>242</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="C84" t="s">
-        <v>54</v>
+        <v>267</v>
       </c>
       <c r="D84" t="s">
         <v>12</v>
@@ -2289,13 +2291,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>64</v>
+        <v>136</v>
       </c>
       <c r="C85" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D85" t="s">
         <v>12</v>
@@ -2303,77 +2305,77 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="C86" t="s">
-        <v>51</v>
+        <v>137</v>
       </c>
       <c r="D86" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
-      <c r="A87" t="s">
-        <v>263</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C87" t="s">
-        <v>148</v>
-      </c>
-      <c r="D87" t="s">
-        <v>12</v>
-      </c>
+    <row r="88" spans="1:4">
+      <c r="A88" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B88" s="4"/>
+      <c r="C88" s="4"/>
+      <c r="D88" s="4"/>
     </row>
     <row r="89" spans="1:4">
-      <c r="A89" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="B89" s="3"/>
-      <c r="C89" s="3"/>
-      <c r="D89" s="3"/>
+      <c r="A89" t="s">
+        <v>245</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C89" t="s">
+        <v>55</v>
+      </c>
+      <c r="D89" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" t="s">
-        <v>264</v>
+        <v>246</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>72</v>
+        <v>132</v>
       </c>
       <c r="C90" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="D90" t="s">
-        <v>12</v>
+        <v>271</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" t="s">
-        <v>265</v>
+        <v>247</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>143</v>
+        <v>95</v>
       </c>
       <c r="C91" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D91" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" t="s">
-        <v>266</v>
+        <v>248</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="C92" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="D92" t="s">
         <v>12</v>
@@ -2381,13 +2383,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C93" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="D93" t="s">
         <v>12</v>
@@ -2395,110 +2397,99 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" t="s">
-        <v>268</v>
+        <v>250</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C94" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D94" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="30">
       <c r="A95" t="s">
-        <v>269</v>
+        <v>251</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C95" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D95" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" ht="30">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
       <c r="A96" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="C96" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D96" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" t="s">
-        <v>271</v>
+        <v>253</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C97" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D97" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" t="s">
-        <v>272</v>
+        <v>254</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C98" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D98" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" t="s">
-        <v>273</v>
+        <v>255</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C99" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D99" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
-      <c r="A100" t="s">
-        <v>274</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C100" t="s">
-        <v>50</v>
-      </c>
-      <c r="D100" t="s">
-        <v>12</v>
-      </c>
+    <row r="126" spans="2:2">
+      <c r="B126" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A88:D88"/>
     <mergeCell ref="A5:D5"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="A89:D89"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A61:D61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2510,7 +2501,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A1:D4"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2523,7 +2514,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
@@ -2532,12 +2523,12 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -2551,7 +2542,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -2565,7 +2556,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -2588,7 +2579,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="A1:D14"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2599,108 +2590,108 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
         <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>269</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
@@ -2711,10 +2702,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
@@ -2725,72 +2716,72 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -2804,7 +2795,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="A1:D7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2817,7 +2808,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
       <c r="B1" t="s">
         <v>17</v>
@@ -2826,12 +2817,12 @@
         <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -2845,7 +2836,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -2854,12 +2845,12 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>165</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -2868,12 +2859,12 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>184</v>
+        <v>166</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -2882,12 +2873,12 @@
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
@@ -2896,12 +2887,12 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>271</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
@@ -2949,7 +2940,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2963,10 +2954,10 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AR: modifiche per la modifica password utente
</commit_message>
<xml_diff>
--- a/RP/Esterni/Analisi dei Requisiti/Requisiti.xlsx
+++ b/RP/Esterni/Analisi dei Requisiti/Requisiti.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="Funzionali" sheetId="1" r:id="rId1"/>
@@ -74,9 +74,6 @@
     <t>Il sistema dovrà essere funzionale presso aziende diverse, anche con caratteristiche molto differenti fra di loro</t>
   </si>
   <si>
-    <t>Il sistema dovrà essere multipiattaforma (per quanto riguarda la parte fissa)</t>
-  </si>
-  <si>
     <t>Il sistema funzionerà su qualsiasi dispositivo dove è presente una \uline{JVM}  versione &gt;= 7.02</t>
   </si>
   <si>
@@ -404,9 +401,6 @@
     <t>Un \uline{Dipendente} potrà visualizzare la password personale</t>
   </si>
   <si>
-    <t>Un \uline{Utente} che ha smarrito la propria password per accedere al sistema potrà recuperarla</t>
-  </si>
-  <si>
     <t>Il sistema permetterà agli \uline{Utenti Autenticati} di effettuare il logout, ma non di terminare l'applicazione</t>
   </si>
   <si>
@@ -830,10 +824,16 @@
     <t>Sarà fornito un manuale ad uso \uline{Amministratore Sicurezza} riguardo le azioni che potrà compiere</t>
   </si>
   <si>
-    <t>Un \uline{Utente} che ha smarrito la password ed ha eseguito la procedura di recupero, la riceverà sulla propria casella di posta elettronica</t>
-  </si>
-  <si>
     <t>Statica</t>
+  </si>
+  <si>
+    <t>Un \uline{Utente} che ha smarrito la password ed ha eseguito la procedura di modifica, la riceverà sulla propria casella di posta elettronica</t>
+  </si>
+  <si>
+    <t>Il sistema dovrà essere multipiattaforma (per quanto riguarda i \unline{dispositivi fissi})</t>
+  </si>
+  <si>
+    <t>Un \uline{Utente} che ha smarrito la propria password per accedere al sistema potrà modificarla</t>
   </si>
 </sst>
 </file>
@@ -877,7 +877,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -890,6 +890,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1187,8 +1190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D126"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1201,7 +1204,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1209,35 +1212,35 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1245,10 +1248,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>171</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>99</v>
+        <v>169</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>98</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
@@ -1259,13 +1262,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>128</v>
+        <v>271</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -1273,13 +1276,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -1287,10 +1290,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
@@ -1301,7 +1304,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1309,10 +1312,10 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C12" t="s">
         <v>13</v>
@@ -1323,10 +1326,10 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C13" t="s">
         <v>13</v>
@@ -1337,10 +1340,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
@@ -1351,10 +1354,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C15" t="s">
         <v>13</v>
@@ -1365,10 +1368,10 @@
     </row>
     <row r="16" spans="1:4" ht="30">
       <c r="A16" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
@@ -1379,10 +1382,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C17" t="s">
         <v>13</v>
@@ -1393,13 +1396,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D18" t="s">
         <v>12</v>
@@ -1407,10 +1410,10 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C19" t="s">
         <v>14</v>
@@ -1421,10 +1424,10 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C20" t="s">
         <v>14</v>
@@ -1435,10 +1438,10 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C21" t="s">
         <v>14</v>
@@ -1449,10 +1452,10 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C22" t="s">
         <v>14</v>
@@ -1463,10 +1466,10 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C23" t="s">
         <v>14</v>
@@ -1477,10 +1480,10 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C24" t="s">
         <v>14</v>
@@ -1491,13 +1494,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D25" t="s">
         <v>12</v>
@@ -1505,13 +1508,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
@@ -1519,13 +1522,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D27" t="s">
         <v>12</v>
@@ -1533,13 +1536,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D28" t="s">
         <v>12</v>
@@ -1547,13 +1550,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D29" t="s">
         <v>12</v>
@@ -1561,13 +1564,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D30" t="s">
         <v>12</v>
@@ -1575,13 +1578,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
@@ -1589,13 +1592,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D32" t="s">
         <v>12</v>
@@ -1603,13 +1606,13 @@
     </row>
     <row r="33" spans="1:4" ht="30">
       <c r="A33" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D33" t="s">
         <v>12</v>
@@ -1617,41 +1620,41 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D34" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="30">
       <c r="A35" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D35" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D36" t="s">
         <v>12</v>
@@ -1659,27 +1662,27 @@
     </row>
     <row r="37" spans="1:4" ht="30">
       <c r="A37" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C37" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D37" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="30">
       <c r="A38" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C38" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D38" t="s">
         <v>12</v>
@@ -1687,13 +1690,13 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C39" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D39" t="s">
         <v>12</v>
@@ -1701,13 +1704,13 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C40" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D40" t="s">
         <v>12</v>
@@ -1715,7 +1718,7 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -1723,10 +1726,10 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C43" t="s">
         <v>14</v>
@@ -1737,97 +1740,97 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C44" t="s">
         <v>14</v>
       </c>
       <c r="D44" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C45" t="s">
         <v>14</v>
       </c>
       <c r="D45" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C46" t="s">
         <v>14</v>
       </c>
       <c r="D46" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C47" t="s">
         <v>14</v>
       </c>
       <c r="D47" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C48" t="s">
         <v>14</v>
       </c>
       <c r="D48" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C49" t="s">
         <v>14</v>
       </c>
       <c r="D49" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C50" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D50" t="s">
         <v>12</v>
@@ -1835,13 +1838,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C51" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D51" t="s">
         <v>12</v>
@@ -1849,13 +1852,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C52" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D52" t="s">
         <v>12</v>
@@ -1863,13 +1866,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C53" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D53" t="s">
         <v>12</v>
@@ -1877,13 +1880,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C54" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D54" t="s">
         <v>12</v>
@@ -1891,13 +1894,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C55" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D55" t="s">
         <v>12</v>
@@ -1905,13 +1908,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C56" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D56" t="s">
         <v>12</v>
@@ -1919,13 +1922,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C57" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D57" t="s">
         <v>12</v>
@@ -1933,13 +1936,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C58" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D58" t="s">
         <v>12</v>
@@ -1947,13 +1950,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C59" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D59" t="s">
         <v>12</v>
@@ -1961,7 +1964,7 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -1969,13 +1972,13 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C62" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D62" t="s">
         <v>12</v>
@@ -1983,13 +1986,13 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C63" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D63" t="s">
         <v>12</v>
@@ -1997,13 +2000,13 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C64" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D64" t="s">
         <v>12</v>
@@ -2011,13 +2014,13 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C65" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D65" t="s">
         <v>12</v>
@@ -2025,13 +2028,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C66" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D66" t="s">
         <v>12</v>
@@ -2039,13 +2042,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C67" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D67" t="s">
         <v>12</v>
@@ -2053,13 +2056,13 @@
     </row>
     <row r="68" spans="1:4" ht="30">
       <c r="A68" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C68" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D68" t="s">
         <v>12</v>
@@ -2067,13 +2070,13 @@
     </row>
     <row r="69" spans="1:4" ht="30">
       <c r="A69" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C69" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D69" t="s">
         <v>12</v>
@@ -2081,13 +2084,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C70" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D70" t="s">
         <v>12</v>
@@ -2095,13 +2098,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C71" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D71" t="s">
         <v>12</v>
@@ -2109,13 +2112,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C72" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D72" t="s">
         <v>12</v>
@@ -2123,13 +2126,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C73" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D73" t="s">
         <v>12</v>
@@ -2137,125 +2140,125 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C74" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D74" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C75" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D75" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C76" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D76" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C77" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D77" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C78" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D78" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="30">
       <c r="A79" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C79" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D79" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C80" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D80" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C81" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D81" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C82" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D82" t="s">
         <v>12</v>
@@ -2263,13 +2266,13 @@
     </row>
     <row r="83" spans="1:4" ht="30">
       <c r="A83" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C83" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D83" t="s">
         <v>12</v>
@@ -2277,13 +2280,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C84" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D84" t="s">
         <v>12</v>
@@ -2291,13 +2294,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C85" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D85" t="s">
         <v>12</v>
@@ -2305,13 +2308,13 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B86" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C86" t="s">
         <v>135</v>
-      </c>
-      <c r="C86" t="s">
-        <v>137</v>
       </c>
       <c r="D86" t="s">
         <v>12</v>
@@ -2319,7 +2322,7 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
@@ -2327,13 +2330,13 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C89" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D89" t="s">
         <v>12</v>
@@ -2341,27 +2344,27 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C90" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D90" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C91" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D91" t="s">
         <v>12</v>
@@ -2369,10 +2372,10 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C92" t="s">
         <v>14</v>
@@ -2383,13 +2386,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C93" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D93" t="s">
         <v>12</v>
@@ -2397,69 +2400,69 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C94" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D94" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="30">
       <c r="A95" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C95" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D95" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C96" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D96" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C97" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D97" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C98" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D98" t="s">
         <v>12</v>
@@ -2467,13 +2470,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C99" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D99" t="s">
         <v>12</v>
@@ -2501,7 +2504,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2514,7 +2517,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
@@ -2523,12 +2526,12 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -2542,7 +2545,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -2556,7 +2559,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -2579,7 +2582,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2590,108 +2593,108 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
         <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B6" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
@@ -2702,10 +2705,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
@@ -2716,72 +2719,72 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -2794,8 +2797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2808,7 +2811,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B1" t="s">
         <v>17</v>
@@ -2817,15 +2820,15 @@
         <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>270</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -2836,63 +2839,63 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
@@ -2940,7 +2943,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2954,10 +2957,10 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Analisi dei Requisiti] Correzione requisiti
</commit_message>
<xml_diff>
--- a/RP/Esterni/Analisi dei Requisiti/Requisiti.xlsx
+++ b/RP/Esterni/Analisi dei Requisiti/Requisiti.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700"/>
@@ -827,20 +827,20 @@
     <t>Statica</t>
   </si>
   <si>
-    <t>Un \uline{Utente} che ha smarrito la password ed ha eseguito la procedura di modifica, la riceverà sulla propria casella di posta elettronica</t>
-  </si>
-  <si>
     <t>Il sistema dovrà essere multipiattaforma (per quanto riguarda i \unline{dispositivi fissi})</t>
   </si>
   <si>
     <t>Un \uline{Utente} che ha smarrito la propria password per accedere al sistema potrà modificarla</t>
+  </si>
+  <si>
+    <t>Un \uline{Utente} che ha smarrito la password ed ha eseguito la procedura di modifica, ne riceverà nella casella di posta, una nuova auto generata randomicamente che dovrà modificare al primo login</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -888,11 +888,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -900,6 +900,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -978,6 +983,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1012,6 +1018,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1187,14 +1194,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="136" style="1" customWidth="1"/>
@@ -1202,15 +1209,15 @@
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>167</v>
       </c>
@@ -1224,7 +1231,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>168</v>
       </c>
@@ -1238,19 +1245,19 @@
         <v>268</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>169</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C6" t="s">
@@ -1260,12 +1267,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>170</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C7" t="s">
         <v>42</v>
@@ -1274,12 +1281,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>171</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C8" t="s">
         <v>42</v>
@@ -1288,7 +1295,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>172</v>
       </c>
@@ -1302,15 +1309,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>173</v>
       </c>
@@ -1324,7 +1331,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>174</v>
       </c>
@@ -1338,7 +1345,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>175</v>
       </c>
@@ -1352,7 +1359,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>176</v>
       </c>
@@ -1366,7 +1373,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30">
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>177</v>
       </c>
@@ -1380,7 +1387,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>178</v>
       </c>
@@ -1394,7 +1401,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>254</v>
       </c>
@@ -1408,7 +1415,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>179</v>
       </c>
@@ -1422,7 +1429,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>180</v>
       </c>
@@ -1436,7 +1443,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>181</v>
       </c>
@@ -1450,7 +1457,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>182</v>
       </c>
@@ -1464,7 +1471,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>183</v>
       </c>
@@ -1478,7 +1485,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>184</v>
       </c>
@@ -1492,7 +1499,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>185</v>
       </c>
@@ -1506,7 +1513,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>186</v>
       </c>
@@ -1520,7 +1527,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>187</v>
       </c>
@@ -1534,7 +1541,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>188</v>
       </c>
@@ -1548,7 +1555,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>189</v>
       </c>
@@ -1562,7 +1569,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>190</v>
       </c>
@@ -1576,7 +1583,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>191</v>
       </c>
@@ -1590,7 +1597,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>192</v>
       </c>
@@ -1604,7 +1611,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="30">
+    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>193</v>
       </c>
@@ -1618,7 +1625,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>194</v>
       </c>
@@ -1632,7 +1639,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30">
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>195</v>
       </c>
@@ -1646,7 +1653,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>196</v>
       </c>
@@ -1660,7 +1667,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="30">
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>197</v>
       </c>
@@ -1674,7 +1681,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="30">
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>198</v>
       </c>
@@ -1688,7 +1695,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>199</v>
       </c>
@@ -1702,7 +1709,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>200</v>
       </c>
@@ -1716,15 +1723,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="4" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>201</v>
       </c>
@@ -1738,7 +1745,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>202</v>
       </c>
@@ -1752,7 +1759,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>203</v>
       </c>
@@ -1766,7 +1773,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>204</v>
       </c>
@@ -1780,7 +1787,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>205</v>
       </c>
@@ -1794,7 +1801,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>206</v>
       </c>
@@ -1808,7 +1815,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>207</v>
       </c>
@@ -1822,7 +1829,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>208</v>
       </c>
@@ -1836,7 +1843,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>209</v>
       </c>
@@ -1850,7 +1857,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>210</v>
       </c>
@@ -1864,7 +1871,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>211</v>
       </c>
@@ -1878,7 +1885,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>212</v>
       </c>
@@ -1892,7 +1899,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>213</v>
       </c>
@@ -1906,7 +1913,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>214</v>
       </c>
@@ -1920,7 +1927,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>215</v>
       </c>
@@ -1934,7 +1941,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>216</v>
       </c>
@@ -1948,7 +1955,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>217</v>
       </c>
@@ -1962,15 +1969,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="4" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B61" s="4"/>
-      <c r="C61" s="4"/>
-      <c r="D61" s="4"/>
-    </row>
-    <row r="62" spans="1:4">
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>218</v>
       </c>
@@ -1984,7 +1991,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>219</v>
       </c>
@@ -1998,7 +2005,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>220</v>
       </c>
@@ -2012,7 +2019,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>221</v>
       </c>
@@ -2026,7 +2033,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>222</v>
       </c>
@@ -2040,7 +2047,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>223</v>
       </c>
@@ -2054,7 +2061,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="30">
+    <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>224</v>
       </c>
@@ -2068,7 +2075,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="30">
+    <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>225</v>
       </c>
@@ -2082,7 +2089,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>226</v>
       </c>
@@ -2096,7 +2103,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>227</v>
       </c>
@@ -2110,7 +2117,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>228</v>
       </c>
@@ -2124,7 +2131,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>229</v>
       </c>
@@ -2138,7 +2145,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>230</v>
       </c>
@@ -2152,7 +2159,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>231</v>
       </c>
@@ -2166,7 +2173,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>232</v>
       </c>
@@ -2180,7 +2187,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>233</v>
       </c>
@@ -2194,7 +2201,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>234</v>
       </c>
@@ -2208,7 +2215,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="30">
+    <row r="79" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>235</v>
       </c>
@@ -2222,7 +2229,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>236</v>
       </c>
@@ -2236,7 +2243,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>237</v>
       </c>
@@ -2250,7 +2257,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>238</v>
       </c>
@@ -2264,7 +2271,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="30">
+    <row r="83" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>239</v>
       </c>
@@ -2278,7 +2285,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>240</v>
       </c>
@@ -2292,7 +2299,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>241</v>
       </c>
@@ -2306,7 +2313,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>242</v>
       </c>
@@ -2320,15 +2327,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
-      <c r="A88" s="4" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B88" s="4"/>
-      <c r="C88" s="4"/>
-      <c r="D88" s="4"/>
-    </row>
-    <row r="89" spans="1:4">
+      <c r="B88" s="5"/>
+      <c r="C88" s="5"/>
+      <c r="D88" s="5"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>243</v>
       </c>
@@ -2342,7 +2349,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>244</v>
       </c>
@@ -2356,7 +2363,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>245</v>
       </c>
@@ -2370,7 +2377,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>246</v>
       </c>
@@ -2384,7 +2391,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>247</v>
       </c>
@@ -2398,7 +2405,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>248</v>
       </c>
@@ -2412,7 +2419,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="30">
+    <row r="95" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>249</v>
       </c>
@@ -2426,7 +2433,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>250</v>
       </c>
@@ -2440,7 +2447,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>251</v>
       </c>
@@ -2454,7 +2461,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>252</v>
       </c>
@@ -2468,7 +2475,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>253</v>
       </c>
@@ -2482,7 +2489,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="126" spans="2:2">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B126" s="3"/>
     </row>
   </sheetData>
@@ -2500,14 +2507,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="93.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
@@ -2515,7 +2522,7 @@
     <col min="5" max="5" width="119" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>142</v>
       </c>
@@ -2529,7 +2536,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>143</v>
       </c>
@@ -2543,7 +2550,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>144</v>
       </c>
@@ -2557,7 +2564,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>145</v>
       </c>
@@ -2578,20 +2585,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="146.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>146</v>
       </c>
@@ -2605,7 +2612,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>147</v>
       </c>
@@ -2619,7 +2626,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>148</v>
       </c>
@@ -2633,7 +2640,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>149</v>
       </c>
@@ -2647,7 +2654,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>150</v>
       </c>
@@ -2661,7 +2668,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>151</v>
       </c>
@@ -2675,7 +2682,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>152</v>
       </c>
@@ -2689,7 +2696,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>153</v>
       </c>
@@ -2703,7 +2710,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>154</v>
       </c>
@@ -2717,7 +2724,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>155</v>
       </c>
@@ -2731,7 +2738,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>156</v>
       </c>
@@ -2745,7 +2752,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>157</v>
       </c>
@@ -2759,7 +2766,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>158</v>
       </c>
@@ -2773,7 +2780,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>159</v>
       </c>
@@ -2794,14 +2801,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="137.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
@@ -2809,7 +2816,7 @@
     <col min="9" max="9" width="162.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>160</v>
       </c>
@@ -2823,12 +2830,12 @@
         <v>268</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>161</v>
       </c>
       <c r="B2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -2837,7 +2844,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>162</v>
       </c>
@@ -2851,7 +2858,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>163</v>
       </c>
@@ -2865,7 +2872,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>164</v>
       </c>
@@ -2879,7 +2886,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>165</v>
       </c>
@@ -2893,7 +2900,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>166</v>
       </c>
@@ -2913,14 +2920,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
@@ -2929,7 +2936,7 @@
     <col min="5" max="5" width="51.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2946,7 +2953,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
AR: cap 4,5 a posto, modificata una immagine UC
</commit_message>
<xml_diff>
--- a/RP/Esterni/Analisi dei Requisiti/Requisiti.xlsx
+++ b/RP/Esterni/Analisi dei Requisiti/Requisiti.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Funzionali" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="199">
   <si>
     <t>Codice</t>
   </si>
@@ -446,345 +446,6 @@
     <t>AMMINISTRATORE INSTALLATORE</t>
   </si>
   <si>
-    <t>RPOB 1</t>
-  </si>
-  <si>
-    <t>RPOB 2</t>
-  </si>
-  <si>
-    <t>RPOB 2.1</t>
-  </si>
-  <si>
-    <t>RPOB 2.2</t>
-  </si>
-  <si>
-    <t>RQOB 1</t>
-  </si>
-  <si>
-    <t>RQOB 2</t>
-  </si>
-  <si>
-    <t>RQOB 2.1</t>
-  </si>
-  <si>
-    <t>RQOB 2.2</t>
-  </si>
-  <si>
-    <t>RQOB 2.3</t>
-  </si>
-  <si>
-    <t>RQOB 2.4</t>
-  </si>
-  <si>
-    <t>RQOB 3</t>
-  </si>
-  <si>
-    <t>RQOP 3.1</t>
-  </si>
-  <si>
-    <t>RQOP 3.2</t>
-  </si>
-  <si>
-    <t>RQOB 4</t>
-  </si>
-  <si>
-    <t>RQD 5</t>
-  </si>
-  <si>
-    <t>RQD 6</t>
-  </si>
-  <si>
-    <t>RQD 6.1</t>
-  </si>
-  <si>
-    <t>RQD 6.2</t>
-  </si>
-  <si>
-    <t>RVOB 1</t>
-  </si>
-  <si>
-    <t>RVOB 1.1</t>
-  </si>
-  <si>
-    <t>RVOB 1.1.1</t>
-  </si>
-  <si>
-    <t>RVOB 1.2</t>
-  </si>
-  <si>
-    <t>RVOB 2</t>
-  </si>
-  <si>
-    <t>RVOB 3</t>
-  </si>
-  <si>
-    <t>RVD 4</t>
-  </si>
-  <si>
-    <t>RFOB 1</t>
-  </si>
-  <si>
-    <t>RFOB 1.1</t>
-  </si>
-  <si>
-    <t>RFOB 2</t>
-  </si>
-  <si>
-    <t>RFOB 3</t>
-  </si>
-  <si>
-    <t>RFOB 3.1</t>
-  </si>
-  <si>
-    <t>RFOB 4</t>
-  </si>
-  <si>
-    <t>RFOB 5</t>
-  </si>
-  <si>
-    <t>RFOB 6</t>
-  </si>
-  <si>
-    <t>RFOB 6.1</t>
-  </si>
-  <si>
-    <t>RFOB 7</t>
-  </si>
-  <si>
-    <t>RFOB 8</t>
-  </si>
-  <si>
-    <t>RFOB 8.1</t>
-  </si>
-  <si>
-    <t>RFOB 9</t>
-  </si>
-  <si>
-    <t>RFOB 9.1</t>
-  </si>
-  <si>
-    <t>RFOB 9.2</t>
-  </si>
-  <si>
-    <t>RFOB 10</t>
-  </si>
-  <si>
-    <t>RFOB 10.1</t>
-  </si>
-  <si>
-    <t>RFOB 10.2</t>
-  </si>
-  <si>
-    <t>RFOB 11</t>
-  </si>
-  <si>
-    <t>RFOB 11.1</t>
-  </si>
-  <si>
-    <t>RFOB 11.2</t>
-  </si>
-  <si>
-    <t>RFOB 11.3</t>
-  </si>
-  <si>
-    <t>RFOB 11.4</t>
-  </si>
-  <si>
-    <t>RFOB 11.5</t>
-  </si>
-  <si>
-    <t>RFOB 11.6</t>
-  </si>
-  <si>
-    <t>RFOB 11.7</t>
-  </si>
-  <si>
-    <t>RFOB 12</t>
-  </si>
-  <si>
-    <t>RFOB 13</t>
-  </si>
-  <si>
-    <t>RFOB 13.1</t>
-  </si>
-  <si>
-    <t>RFOB 14</t>
-  </si>
-  <si>
-    <t>RFOB 14.1</t>
-  </si>
-  <si>
-    <t>RFOB 14.2</t>
-  </si>
-  <si>
-    <t>RFOB 14.2.1</t>
-  </si>
-  <si>
-    <t>RFOB 14.2.2</t>
-  </si>
-  <si>
-    <t>RFOB 15</t>
-  </si>
-  <si>
-    <t>RFOB 15.1</t>
-  </si>
-  <si>
-    <t>RFOB 15.1.1</t>
-  </si>
-  <si>
-    <t>RFOB 15.1.2</t>
-  </si>
-  <si>
-    <t>RFOB 15.1.3</t>
-  </si>
-  <si>
-    <t>RFOB 15.1.4</t>
-  </si>
-  <si>
-    <t>RFOB 15.1.5</t>
-  </si>
-  <si>
-    <t>RFOB 16</t>
-  </si>
-  <si>
-    <t>RFOB 16.1</t>
-  </si>
-  <si>
-    <t>RFOB 16.2</t>
-  </si>
-  <si>
-    <t>RFOB 16.3</t>
-  </si>
-  <si>
-    <t>RFOB 16.4</t>
-  </si>
-  <si>
-    <t>RFOB 16.5</t>
-  </si>
-  <si>
-    <t>RFOB 17</t>
-  </si>
-  <si>
-    <t>RFOB 18</t>
-  </si>
-  <si>
-    <t>RFOB 18.1</t>
-  </si>
-  <si>
-    <t>RFOB 19</t>
-  </si>
-  <si>
-    <t>RFOB 20</t>
-  </si>
-  <si>
-    <t>RFOB 20.1</t>
-  </si>
-  <si>
-    <t>RFOB 20.2</t>
-  </si>
-  <si>
-    <t>RFOB 20.3</t>
-  </si>
-  <si>
-    <t>RFOB 20.4</t>
-  </si>
-  <si>
-    <t>RFOB 20.5</t>
-  </si>
-  <si>
-    <t>RFOB 20.6</t>
-  </si>
-  <si>
-    <t>RFOB 20.7</t>
-  </si>
-  <si>
-    <t>RFOB 20.8</t>
-  </si>
-  <si>
-    <t>RFOB 20.9</t>
-  </si>
-  <si>
-    <t>RFOB 21</t>
-  </si>
-  <si>
-    <t>RFOB 21.1</t>
-  </si>
-  <si>
-    <t>RFOB 21.1.1</t>
-  </si>
-  <si>
-    <t>RFOB 21.1.2</t>
-  </si>
-  <si>
-    <t>RFOB 21.1.3</t>
-  </si>
-  <si>
-    <t>RFOB 21.1.4</t>
-  </si>
-  <si>
-    <t>RFOB 21.1.5</t>
-  </si>
-  <si>
-    <t>RFOB 21.1.6</t>
-  </si>
-  <si>
-    <t>RFOB 21.1.7</t>
-  </si>
-  <si>
-    <t>RFOB 21.1.8</t>
-  </si>
-  <si>
-    <t>RFOB 21.2</t>
-  </si>
-  <si>
-    <t>RFOB 21.2.1</t>
-  </si>
-  <si>
-    <t>RFOB 21.3</t>
-  </si>
-  <si>
-    <t>RFOB 22</t>
-  </si>
-  <si>
-    <t>RFOB 23</t>
-  </si>
-  <si>
-    <t>RFOB 24</t>
-  </si>
-  <si>
-    <t>RFOB 25</t>
-  </si>
-  <si>
-    <t>RFOB 26</t>
-  </si>
-  <si>
-    <t>RFOB 27</t>
-  </si>
-  <si>
-    <t>RFOB 27.1</t>
-  </si>
-  <si>
-    <t>RFOB 27.1.1</t>
-  </si>
-  <si>
-    <t>RFOB 27.1.2</t>
-  </si>
-  <si>
-    <t>RFOB 27.1.3</t>
-  </si>
-  <si>
-    <t>RFOB 27.1.4</t>
-  </si>
-  <si>
-    <t>RFOB 27.2</t>
-  </si>
-  <si>
-    <t>RFOB 27.3</t>
-  </si>
-  <si>
-    <t>RFD 8.2</t>
-  </si>
-  <si>
     <t>Il modulo di registrazione richiederà i dati personali del \uline{Dipendente}</t>
   </si>
   <si>
@@ -834,13 +495,133 @@
   </si>
   <si>
     <t>Un \uline{Utente} che ha smarrito la password ed ha eseguito la procedura di modifica, ne riceverà nella casella di posta, una nuova auto generata randomicamente che dovrà modificare al primo login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RFOB </t>
+  </si>
+  <si>
+    <t>RFOB .1</t>
+  </si>
+  <si>
+    <t>RFD .2</t>
+  </si>
+  <si>
+    <t>RFOB .2</t>
+  </si>
+  <si>
+    <t>RFOB .3</t>
+  </si>
+  <si>
+    <t>RFOB .4</t>
+  </si>
+  <si>
+    <t>RFOB .5</t>
+  </si>
+  <si>
+    <t>RFOB .6</t>
+  </si>
+  <si>
+    <t>RFOB .7</t>
+  </si>
+  <si>
+    <t>RFOB .2.1</t>
+  </si>
+  <si>
+    <t>RFOB .2.2</t>
+  </si>
+  <si>
+    <t>RFOB .1.1</t>
+  </si>
+  <si>
+    <t>RFOB .1.2</t>
+  </si>
+  <si>
+    <t>RFOB .1.3</t>
+  </si>
+  <si>
+    <t>RFOB .1.4</t>
+  </si>
+  <si>
+    <t>RFOB .1.5</t>
+  </si>
+  <si>
+    <t>RFOB .8</t>
+  </si>
+  <si>
+    <t>RFOB .9</t>
+  </si>
+  <si>
+    <t>RFOB .1.6</t>
+  </si>
+  <si>
+    <t>RFOB .1.7</t>
+  </si>
+  <si>
+    <t>RFOB .1.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPOB </t>
+  </si>
+  <si>
+    <t>RPOB .1</t>
+  </si>
+  <si>
+    <t>RPOB .2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RQOB </t>
+  </si>
+  <si>
+    <t>RQOB</t>
+  </si>
+  <si>
+    <t>RQOB .1</t>
+  </si>
+  <si>
+    <t>RQOB .2</t>
+  </si>
+  <si>
+    <t>RQOB .3</t>
+  </si>
+  <si>
+    <t>RQOB .4</t>
+  </si>
+  <si>
+    <t>RQOP .1</t>
+  </si>
+  <si>
+    <t>RQOP .2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RQD </t>
+  </si>
+  <si>
+    <t>RQD .1</t>
+  </si>
+  <si>
+    <t>RQD .2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RVOB </t>
+  </si>
+  <si>
+    <t>RVOB .1</t>
+  </si>
+  <si>
+    <t>RVOB .1.1</t>
+  </si>
+  <si>
+    <t>RVOB .2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RVD </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -877,7 +658,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -894,6 +675,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -983,7 +765,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1018,7 +799,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1194,14 +974,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="136" style="1" customWidth="1"/>
@@ -1209,7 +989,7 @@
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="5" t="s">
         <v>137</v>
       </c>
@@ -1217,9 +997,9 @@
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>56</v>
@@ -1228,12 +1008,12 @@
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>55</v>
@@ -1242,10 +1022,10 @@
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="5" t="s">
         <v>136</v>
       </c>
@@ -1253,9 +1033,9 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>98</v>
@@ -1267,12 +1047,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>270</v>
+        <v>157</v>
       </c>
       <c r="C7" t="s">
         <v>42</v>
@@ -1281,12 +1061,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="30">
       <c r="A8" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>271</v>
+        <v>158</v>
       </c>
       <c r="C8" t="s">
         <v>42</v>
@@ -1295,9 +1075,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>127</v>
@@ -1309,7 +1089,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="5" t="s">
         <v>138</v>
       </c>
@@ -1317,9 +1097,9 @@
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>95</v>
@@ -1331,9 +1111,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>96</v>
@@ -1345,9 +1125,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>97</v>
@@ -1359,9 +1139,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>99</v>
@@ -1373,9 +1153,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="30">
       <c r="A16" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>100</v>
@@ -1387,9 +1167,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>101</v>
@@ -1401,9 +1181,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>254</v>
+        <v>161</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>102</v>
@@ -1415,9 +1195,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>114</v>
@@ -1429,9 +1209,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>115</v>
@@ -1443,9 +1223,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>116</v>
@@ -1457,9 +1237,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>182</v>
+        <v>159</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>117</v>
@@ -1471,9 +1251,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>183</v>
+        <v>160</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>118</v>
@@ -1485,9 +1265,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>184</v>
+        <v>162</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>119</v>
@@ -1499,9 +1279,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>185</v>
+        <v>159</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>120</v>
@@ -1513,9 +1293,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>186</v>
+        <v>160</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>121</v>
@@ -1527,9 +1307,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>187</v>
+        <v>162</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>122</v>
@@ -1541,9 +1321,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>188</v>
+        <v>163</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>123</v>
@@ -1555,9 +1335,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>124</v>
@@ -1569,9 +1349,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>190</v>
+        <v>165</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>125</v>
@@ -1583,9 +1363,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>191</v>
+        <v>166</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>126</v>
@@ -1597,9 +1377,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>192</v>
+        <v>167</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>129</v>
@@ -1611,9 +1391,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="30">
       <c r="A33" t="s">
-        <v>193</v>
+        <v>159</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>59</v>
@@ -1625,9 +1405,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>194</v>
+        <v>159</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>60</v>
@@ -1636,12 +1416,12 @@
         <v>52</v>
       </c>
       <c r="D34" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="30">
       <c r="A35" t="s">
-        <v>195</v>
+        <v>160</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>61</v>
@@ -1650,12 +1430,12 @@
         <v>50</v>
       </c>
       <c r="D35" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>196</v>
+        <v>159</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>62</v>
@@ -1667,9 +1447,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="30">
       <c r="A37" t="s">
-        <v>197</v>
+        <v>160</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>63</v>
@@ -1678,12 +1458,12 @@
         <v>51</v>
       </c>
       <c r="D37" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="30">
       <c r="A38" t="s">
-        <v>198</v>
+        <v>162</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>104</v>
@@ -1695,9 +1475,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>199</v>
+        <v>168</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>105</v>
@@ -1709,9 +1489,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>200</v>
+        <v>169</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>106</v>
@@ -1723,7 +1503,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="A42" s="5" t="s">
         <v>139</v>
       </c>
@@ -1731,9 +1511,9 @@
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>201</v>
+        <v>159</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>103</v>
@@ -1745,93 +1525,93 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>202</v>
+        <v>160</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>255</v>
+        <v>142</v>
       </c>
       <c r="C44" t="s">
         <v>14</v>
       </c>
       <c r="D44" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>203</v>
+        <v>170</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>256</v>
+        <v>143</v>
       </c>
       <c r="C45" t="s">
         <v>14</v>
       </c>
       <c r="D45" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>204</v>
+        <v>171</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>257</v>
+        <v>144</v>
       </c>
       <c r="C46" t="s">
         <v>14</v>
       </c>
       <c r="D46" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>205</v>
+        <v>172</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>258</v>
+        <v>145</v>
       </c>
       <c r="C47" t="s">
         <v>14</v>
       </c>
       <c r="D47" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>206</v>
+        <v>173</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>259</v>
+        <v>146</v>
       </c>
       <c r="C48" t="s">
         <v>14</v>
       </c>
       <c r="D48" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>207</v>
+        <v>174</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>260</v>
+        <v>147</v>
       </c>
       <c r="C49" t="s">
         <v>14</v>
       </c>
       <c r="D49" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>208</v>
+        <v>159</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>107</v>
@@ -1843,9 +1623,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>209</v>
+        <v>160</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>108</v>
@@ -1857,9 +1637,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>210</v>
+        <v>162</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>109</v>
@@ -1871,9 +1651,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>211</v>
+        <v>163</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>110</v>
@@ -1885,9 +1665,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>212</v>
+        <v>164</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>111</v>
@@ -1899,9 +1679,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>213</v>
+        <v>165</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>112</v>
@@ -1913,9 +1693,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>214</v>
+        <v>159</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>113</v>
@@ -1927,12 +1707,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>215</v>
+        <v>159</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>261</v>
+        <v>148</v>
       </c>
       <c r="C57" t="s">
         <v>53</v>
@@ -1941,9 +1721,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>216</v>
+        <v>160</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>64</v>
@@ -1955,9 +1735,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>217</v>
+        <v>159</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>66</v>
@@ -1969,7 +1749,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4">
       <c r="A61" s="5" t="s">
         <v>140</v>
       </c>
@@ -1977,9 +1757,9 @@
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>218</v>
+        <v>159</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>85</v>
@@ -1991,9 +1771,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>219</v>
+        <v>160</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>84</v>
@@ -2005,9 +1785,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>220</v>
+        <v>162</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>83</v>
@@ -2019,9 +1799,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>221</v>
+        <v>163</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>82</v>
@@ -2033,9 +1813,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>222</v>
+        <v>164</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>81</v>
@@ -2047,9 +1827,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>223</v>
+        <v>165</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>80</v>
@@ -2061,12 +1841,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="30">
       <c r="A68" t="s">
-        <v>224</v>
+        <v>166</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>262</v>
+        <v>149</v>
       </c>
       <c r="C68" t="s">
         <v>131</v>
@@ -2075,9 +1855,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="30">
       <c r="A69" t="s">
-        <v>225</v>
+        <v>167</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>79</v>
@@ -2089,9 +1869,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>226</v>
+        <v>175</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>78</v>
@@ -2103,9 +1883,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>227</v>
+        <v>176</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>77</v>
@@ -2117,9 +1897,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>228</v>
+        <v>159</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>76</v>
@@ -2131,177 +1911,177 @@
         <v>12</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>229</v>
+        <v>160</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C73" t="s">
-        <v>264</v>
+        <v>151</v>
       </c>
       <c r="D73" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>230</v>
+        <v>170</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C74" t="s">
-        <v>264</v>
+        <v>151</v>
       </c>
       <c r="D74" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>231</v>
+        <v>171</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C75" t="s">
-        <v>264</v>
+        <v>151</v>
       </c>
       <c r="D75" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>232</v>
+        <v>172</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C76" t="s">
-        <v>264</v>
+        <v>151</v>
       </c>
       <c r="D76" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>233</v>
+        <v>173</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C77" t="s">
-        <v>264</v>
+        <v>151</v>
       </c>
       <c r="D77" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>234</v>
+        <v>174</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C78" t="s">
-        <v>264</v>
+        <v>151</v>
       </c>
       <c r="D78" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="30">
       <c r="A79" t="s">
-        <v>235</v>
+        <v>177</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>263</v>
+        <v>150</v>
       </c>
       <c r="C79" t="s">
-        <v>264</v>
+        <v>151</v>
       </c>
       <c r="D79" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>236</v>
+        <v>178</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>69</v>
       </c>
       <c r="C80" t="s">
-        <v>264</v>
+        <v>151</v>
       </c>
       <c r="D80" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>237</v>
+        <v>179</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>68</v>
       </c>
       <c r="C81" t="s">
-        <v>264</v>
+        <v>151</v>
       </c>
       <c r="D81" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>238</v>
+        <v>162</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C82" t="s">
-        <v>266</v>
+        <v>153</v>
       </c>
       <c r="D82" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" ht="30">
       <c r="A83" t="s">
-        <v>239</v>
+        <v>168</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>57</v>
       </c>
       <c r="C83" t="s">
-        <v>266</v>
+        <v>153</v>
       </c>
       <c r="D83" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>240</v>
+        <v>163</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C84" t="s">
-        <v>265</v>
+        <v>152</v>
       </c>
       <c r="D84" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>241</v>
+        <v>159</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>134</v>
@@ -2313,9 +2093,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4">
       <c r="A86" t="s">
-        <v>242</v>
+        <v>159</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>133</v>
@@ -2327,7 +2107,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4">
       <c r="A88" s="5" t="s">
         <v>141</v>
       </c>
@@ -2335,9 +2115,9 @@
       <c r="C88" s="5"/>
       <c r="D88" s="5"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4">
       <c r="A89" t="s">
-        <v>243</v>
+        <v>159</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>65</v>
@@ -2349,9 +2129,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4">
       <c r="A90" t="s">
-        <v>244</v>
+        <v>159</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>130</v>
@@ -2360,12 +2140,12 @@
         <v>44</v>
       </c>
       <c r="D90" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
       <c r="A91" t="s">
-        <v>245</v>
+        <v>159</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>94</v>
@@ -2377,9 +2157,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4">
       <c r="A92" t="s">
-        <v>246</v>
+        <v>159</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>93</v>
@@ -2391,9 +2171,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4">
       <c r="A93" t="s">
-        <v>247</v>
+        <v>160</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>92</v>
@@ -2405,9 +2185,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4">
       <c r="A94" t="s">
-        <v>248</v>
+        <v>170</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>91</v>
@@ -2416,12 +2196,12 @@
         <v>45</v>
       </c>
       <c r="D94" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="30">
       <c r="A95" t="s">
-        <v>249</v>
+        <v>171</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>90</v>
@@ -2430,12 +2210,12 @@
         <v>45</v>
       </c>
       <c r="D95" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
       <c r="A96" t="s">
-        <v>250</v>
+        <v>172</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>89</v>
@@ -2444,12 +2224,12 @@
         <v>45</v>
       </c>
       <c r="D96" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
       <c r="A97" t="s">
-        <v>251</v>
+        <v>173</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>88</v>
@@ -2458,12 +2238,12 @@
         <v>45</v>
       </c>
       <c r="D97" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
       <c r="A98" t="s">
-        <v>252</v>
+        <v>162</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>87</v>
@@ -2475,9 +2255,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4">
       <c r="A99" t="s">
-        <v>253</v>
+        <v>163</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>86</v>
@@ -2489,7 +2269,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:2">
       <c r="B126" s="3"/>
     </row>
   </sheetData>
@@ -2507,14 +2287,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="93.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
@@ -2522,9 +2302,9 @@
     <col min="5" max="5" width="119" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>142</v>
+        <v>180</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
@@ -2533,12 +2313,12 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>143</v>
+        <v>180</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -2550,9 +2330,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>181</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -2564,9 +2344,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>145</v>
+        <v>182</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -2585,22 +2365,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="146.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>146</v>
+        <v>183</v>
       </c>
       <c r="B1" t="s">
         <v>27</v>
@@ -2609,12 +2389,12 @@
         <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>147</v>
+        <v>184</v>
       </c>
       <c r="B2" t="s">
         <v>26</v>
@@ -2623,12 +2403,12 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>148</v>
+        <v>185</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
@@ -2637,12 +2417,12 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>149</v>
+        <v>186</v>
       </c>
       <c r="B4" t="s">
         <v>24</v>
@@ -2651,12 +2431,12 @@
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>150</v>
+        <v>187</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
@@ -2665,26 +2445,26 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>151</v>
+        <v>188</v>
       </c>
       <c r="B6" t="s">
-        <v>267</v>
+        <v>154</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>152</v>
+        <v>183</v>
       </c>
       <c r="B7" t="s">
         <v>28</v>
@@ -2693,12 +2473,12 @@
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>153</v>
+        <v>189</v>
       </c>
       <c r="B8" t="s">
         <v>29</v>
@@ -2710,9 +2490,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>154</v>
+        <v>190</v>
       </c>
       <c r="B9" t="s">
         <v>30</v>
@@ -2724,9 +2504,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>155</v>
+        <v>183</v>
       </c>
       <c r="B10" t="s">
         <v>31</v>
@@ -2735,12 +2515,12 @@
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
       <c r="B11" t="s">
         <v>32</v>
@@ -2749,12 +2529,12 @@
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>157</v>
+        <v>191</v>
       </c>
       <c r="B12" t="s">
         <v>33</v>
@@ -2763,12 +2543,12 @@
         <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>158</v>
+        <v>192</v>
       </c>
       <c r="B13" t="s">
         <v>34</v>
@@ -2777,12 +2557,12 @@
         <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>159</v>
+        <v>193</v>
       </c>
       <c r="B14" t="s">
         <v>35</v>
@@ -2791,7 +2571,7 @@
         <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>268</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -2801,14 +2581,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="137.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
@@ -2816,9 +2596,9 @@
     <col min="9" max="9" width="162.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>160</v>
+        <v>194</v>
       </c>
       <c r="B1" t="s">
         <v>17</v>
@@ -2827,15 +2607,15 @@
         <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>195</v>
       </c>
       <c r="B2" t="s">
-        <v>269</v>
+        <v>156</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -2844,9 +2624,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>196</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -2855,12 +2635,12 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>163</v>
+        <v>197</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
@@ -2869,12 +2649,12 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>164</v>
+        <v>194</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -2883,12 +2663,12 @@
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>165</v>
+        <v>194</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
@@ -2897,12 +2677,12 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>166</v>
+        <v>198</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
@@ -2914,20 +2694,24 @@
         <v>12</v>
       </c>
     </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
@@ -2936,7 +2720,7 @@
     <col min="5" max="5" width="51.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2953,7 +2737,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
AR: correzioni cap 3, e xlsx. cap 4 a posto
</commit_message>
<xml_diff>
--- a/RP/Esterni/Analisi dei Requisiti/Requisiti.xlsx
+++ b/RP/Esterni/Analisi dei Requisiti/Requisiti.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Funzionali" sheetId="1" r:id="rId1"/>
@@ -80,12 +80,6 @@
     <t>Test / Dinamica</t>
   </si>
   <si>
-    <t>Sarà fornito un manuale ad uso \uline{Amministratore Installatore} riguardo l'installazione del prodotto</t>
-  </si>
-  <si>
-    <t>Sarà fornito un manuale ad uso \uline{Amministratore Azienda}  riguardo tutte le azioni che tale \uline{Utente} potrà compiere</t>
-  </si>
-  <si>
     <t>Sarà fornito un manuale ad uso dei \uline{Dipendenti} che coprirà gli aspetti di utilizzo del software dal loro punto di vista</t>
   </si>
   <si>
@@ -477,6 +471,12 @@
   </si>
   <si>
     <t>Un \uline{Amministratore Installatore} potrà installare il software sui \uline{dispositivi mobili} in un'azienda</t>
+  </si>
+  <si>
+    <t>Sarà fornito un manuale ad uso \uline{Amministratore Azienda}  riguardo tutte le azioni che potrà compiere</t>
+  </si>
+  <si>
+    <t>Sarà fornito un manuale ad uso \uline{Amministratore Installatore} riguardo alle azioni che potrà compiere</t>
   </si>
 </sst>
 </file>
@@ -533,10 +533,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -839,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62:D62"/>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -852,55 +852,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
+      <c r="A1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
+      <c r="A5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -911,13 +911,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -925,60 +925,60 @@
     </row>
     <row r="8" spans="1:4" ht="30">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="6" t="s">
-        <v>59</v>
-      </c>
       <c r="B12" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
@@ -989,10 +989,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
@@ -1003,10 +1003,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
@@ -1017,10 +1017,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
@@ -1031,10 +1031,10 @@
     </row>
     <row r="17" spans="1:4" ht="30">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C17" t="s">
         <v>10</v>
@@ -1045,10 +1045,10 @@
     </row>
     <row r="18" spans="1:4" ht="30">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C18" t="s">
         <v>10</v>
@@ -1059,13 +1059,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D19" t="s">
         <v>9</v>
@@ -1073,10 +1073,10 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C20" t="s">
         <v>10</v>
@@ -1087,10 +1087,10 @@
     </row>
     <row r="21" spans="1:4" ht="30">
       <c r="A21" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C21" t="s">
         <v>10</v>
@@ -1101,10 +1101,10 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C22" t="s">
         <v>10</v>
@@ -1115,10 +1115,10 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C23" t="s">
         <v>11</v>
@@ -1129,10 +1129,10 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C24" t="s">
         <v>11</v>
@@ -1143,10 +1143,10 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C25" t="s">
         <v>11</v>
@@ -1157,10 +1157,10 @@
     </row>
     <row r="26" spans="1:4" ht="30">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C26" t="s">
         <v>11</v>
@@ -1171,13 +1171,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C27" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D27" t="s">
         <v>9</v>
@@ -1185,13 +1185,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C28" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D28" t="s">
         <v>9</v>
@@ -1199,13 +1199,13 @@
     </row>
     <row r="29" spans="1:4" ht="30">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C29" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D29" t="s">
         <v>9</v>
@@ -1213,41 +1213,41 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C30" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D30" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="30">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C31" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D31" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C32" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D32" t="s">
         <v>9</v>
@@ -1255,27 +1255,27 @@
     </row>
     <row r="33" spans="1:4" ht="30">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C33" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D33" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C34" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D34" t="s">
         <v>9</v>
@@ -1283,13 +1283,13 @@
     </row>
     <row r="35" spans="1:4" ht="30">
       <c r="A35" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C35" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D35" t="s">
         <v>9</v>
@@ -1297,13 +1297,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" t="s">
         <v>40</v>
-      </c>
-      <c r="C36" t="s">
-        <v>42</v>
       </c>
       <c r="D36" t="s">
         <v>9</v>
@@ -1311,63 +1311,63 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C37" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D37" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
+      <c r="A39" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="6" t="s">
-        <v>86</v>
+      <c r="A40" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D40" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="6" t="s">
-        <v>86</v>
+      <c r="A41" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>54</v>
+        <v>127</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C42" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D42" t="s">
         <v>9</v>
@@ -1375,13 +1375,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C43" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D43" t="s">
         <v>9</v>
@@ -1389,13 +1389,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C44" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D44" t="s">
         <v>9</v>
@@ -1403,13 +1403,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C45" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D45" t="s">
         <v>9</v>
@@ -1417,13 +1417,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C46" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D46" t="s">
         <v>9</v>
@@ -1431,13 +1431,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C47" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D47" t="s">
         <v>9</v>
@@ -1445,13 +1445,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C48" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D48" t="s">
         <v>9</v>
@@ -1459,13 +1459,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C49" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D49" t="s">
         <v>9</v>
@@ -1473,13 +1473,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C50" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D50" t="s">
         <v>9</v>
@@ -1487,49 +1487,49 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C51" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D51" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
+      <c r="A53" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B53" s="6"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="6" t="s">
-        <v>86</v>
+      <c r="A54" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D54" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D54" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C55" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D55" t="s">
         <v>9</v>
@@ -1537,13 +1537,13 @@
     </row>
     <row r="56" spans="1:4" ht="30">
       <c r="A56" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C56" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D56" t="s">
         <v>9</v>
@@ -1551,13 +1551,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C57" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D57" t="s">
         <v>9</v>
@@ -1565,13 +1565,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C58" t="s">
         <v>139</v>
-      </c>
-      <c r="C58" t="s">
-        <v>141</v>
       </c>
       <c r="D58" t="s">
         <v>9</v>
@@ -1579,13 +1579,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C59" t="s">
         <v>140</v>
-      </c>
-      <c r="C59" t="s">
-        <v>142</v>
       </c>
       <c r="D59" t="s">
         <v>9</v>
@@ -1593,60 +1593,60 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C60" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D60" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B62" s="5"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
+      <c r="A62" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C63" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D63" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C64" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D64" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C65" t="s">
         <v>11</v>
@@ -1657,10 +1657,10 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C66" t="s">
         <v>11</v>
@@ -1671,10 +1671,10 @@
     </row>
     <row r="67" spans="1:4" ht="30">
       <c r="A67" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C67" t="s">
         <v>11</v>
@@ -1718,7 +1718,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
@@ -1727,15 +1727,15 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -1755,7 +1755,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1766,108 +1766,108 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
         <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>151</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>152</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -1878,10 +1878,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -1892,72 +1892,72 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B14" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1970,7 +1970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -1984,7 +1984,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B1" t="s">
         <v>14</v>
@@ -1993,15 +1993,15 @@
         <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -2012,7 +2012,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
@@ -2021,12 +2021,12 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
@@ -2035,12 +2035,12 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
@@ -2049,12 +2049,12 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
@@ -2063,12 +2063,12 @@
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
@@ -2120,7 +2120,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2137,7 +2137,7 @@
         <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AR c 3,4,5 + xlsx
</commit_message>
<xml_diff>
--- a/RP/Esterni/Analisi dei Requisiti/Requisiti.xlsx
+++ b/RP/Esterni/Analisi dei Requisiti/Requisiti.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="Funzionali" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="152">
   <si>
     <t>Codice</t>
   </si>
@@ -131,18 +131,12 @@
     <t>Una proposta di domanda dovrà essere completamente non \uline{invadente}</t>
   </si>
   <si>
-    <t>Tutte le azioni di tutti gli \uline{Utenti}, nel tempo, dovranno essere registrate nel sistema</t>
-  </si>
-  <si>
     <t>Il sistema invia all'indirizzo email del nuovo \uline{Dipendente} la sua username</t>
   </si>
   <si>
     <t>Il sistema invia all'indirizzo email del nuovo \uline{Dipendente} la sua password</t>
   </si>
   <si>
-    <t>UCAA 1.1</t>
-  </si>
-  <si>
     <t>UCASA 2</t>
   </si>
   <si>
@@ -477,6 +471,9 @@
   </si>
   <si>
     <t>Sarà fornito un manuale ad uso \uline{Amministratore Installatore} riguardo alle azioni che potrà compiere</t>
+  </si>
+  <si>
+    <t>Tutte le azioni di tutti gli \uline{utilizzatori}, nel tempo, dovranno essere registrate nel sistema</t>
   </si>
 </sst>
 </file>
@@ -520,15 +517,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -839,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:D67"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -852,16 +846,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="A1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>33</v>
@@ -870,12 +864,12 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>32</v>
@@ -884,23 +878,23 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
+      <c r="A5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>37</v>
+        <v>54</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -911,13 +905,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -925,60 +919,60 @@
     </row>
     <row r="8" spans="1:4" ht="30">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="B12" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
@@ -989,10 +983,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>87</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
@@ -1003,10 +997,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
@@ -1017,10 +1011,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
@@ -1031,10 +1025,10 @@
     </row>
     <row r="17" spans="1:4" ht="30">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C17" t="s">
         <v>10</v>
@@ -1045,10 +1039,10 @@
     </row>
     <row r="18" spans="1:4" ht="30">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C18" t="s">
         <v>10</v>
@@ -1059,10 +1053,10 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C19" t="s">
         <v>25</v>
@@ -1073,10 +1067,10 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C20" t="s">
         <v>10</v>
@@ -1087,10 +1081,10 @@
     </row>
     <row r="21" spans="1:4" ht="30">
       <c r="A21" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C21" t="s">
         <v>10</v>
@@ -1101,10 +1095,10 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C22" t="s">
         <v>10</v>
@@ -1115,10 +1109,10 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C23" t="s">
         <v>11</v>
@@ -1129,10 +1123,10 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C24" t="s">
         <v>11</v>
@@ -1143,10 +1137,10 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C25" t="s">
         <v>11</v>
@@ -1157,10 +1151,10 @@
     </row>
     <row r="26" spans="1:4" ht="30">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C26" t="s">
         <v>11</v>
@@ -1171,13 +1165,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C27" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D27" t="s">
         <v>9</v>
@@ -1185,13 +1179,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C28" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D28" t="s">
         <v>9</v>
@@ -1199,13 +1193,13 @@
     </row>
     <row r="29" spans="1:4" ht="30">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C29" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D29" t="s">
         <v>9</v>
@@ -1213,41 +1207,41 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C30" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D30" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="30">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C31" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D31" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C32" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D32" t="s">
         <v>9</v>
@@ -1255,27 +1249,27 @@
     </row>
     <row r="33" spans="1:4" ht="30">
       <c r="A33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C33" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D33" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C34" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D34" t="s">
         <v>9</v>
@@ -1283,13 +1277,13 @@
     </row>
     <row r="35" spans="1:4" ht="30">
       <c r="A35" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C35" t="s">
-        <v>40</v>
+        <v>129</v>
       </c>
       <c r="D35" t="s">
         <v>9</v>
@@ -1297,13 +1291,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C36" t="s">
-        <v>40</v>
+        <v>129</v>
       </c>
       <c r="D36" t="s">
         <v>9</v>
@@ -1311,63 +1305,63 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C37" t="s">
-        <v>40</v>
+        <v>129</v>
       </c>
       <c r="D37" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
+      <c r="A39" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="5" t="s">
-        <v>84</v>
+      <c r="A40" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="D40" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D40" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="5" t="s">
-        <v>84</v>
+      <c r="A41" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>52</v>
+        <v>125</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C42" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D42" t="s">
         <v>9</v>
@@ -1375,13 +1369,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C43" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D43" t="s">
         <v>9</v>
@@ -1389,13 +1383,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C44" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D44" t="s">
         <v>9</v>
@@ -1403,13 +1397,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C45" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D45" t="s">
         <v>9</v>
@@ -1417,13 +1411,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C46" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D46" t="s">
         <v>9</v>
@@ -1431,13 +1425,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C47" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D47" t="s">
         <v>9</v>
@@ -1445,13 +1439,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C48" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D48" t="s">
         <v>9</v>
@@ -1459,13 +1453,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C49" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D49" t="s">
         <v>9</v>
@@ -1473,13 +1467,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C50" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D50" t="s">
         <v>9</v>
@@ -1487,49 +1481,49 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C51" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D51" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
+      <c r="A53" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="5" t="s">
-        <v>84</v>
+      <c r="A54" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C54" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C54" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="D54" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C55" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D55" t="s">
         <v>9</v>
@@ -1537,13 +1531,13 @@
     </row>
     <row r="56" spans="1:4" ht="30">
       <c r="A56" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C56" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D56" t="s">
         <v>9</v>
@@ -1551,13 +1545,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C57" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D57" t="s">
         <v>9</v>
@@ -1565,13 +1559,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C58" t="s">
         <v>137</v>
-      </c>
-      <c r="C58" t="s">
-        <v>139</v>
       </c>
       <c r="D58" t="s">
         <v>9</v>
@@ -1579,13 +1573,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C59" t="s">
         <v>138</v>
-      </c>
-      <c r="C59" t="s">
-        <v>140</v>
       </c>
       <c r="D59" t="s">
         <v>9</v>
@@ -1593,60 +1587,60 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C60" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D60" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B62" s="6"/>
-      <c r="C62" s="6"/>
-      <c r="D62" s="6"/>
+      <c r="A62" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C63" t="s">
         <v>31</v>
       </c>
       <c r="D63" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C64" t="s">
         <v>28</v>
       </c>
       <c r="D64" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C65" t="s">
         <v>11</v>
@@ -1657,10 +1651,10 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C66" t="s">
         <v>11</v>
@@ -1671,10 +1665,10 @@
     </row>
     <row r="67" spans="1:4" ht="30">
       <c r="A67" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C67" t="s">
         <v>11</v>
@@ -1718,7 +1712,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
@@ -1727,15 +1721,15 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -1766,7 +1760,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
         <v>22</v>
@@ -1775,12 +1769,12 @@
         <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
         <v>21</v>
@@ -1789,12 +1783,12 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
@@ -1803,54 +1797,54 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
         <v>23</v>
@@ -1859,15 +1853,15 @@
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -1878,10 +1872,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -1892,21 +1886,21 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B11" t="s">
         <v>24</v>
@@ -1915,49 +1909,49 @@
         <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B14" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1970,7 +1964,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -1984,7 +1978,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
         <v>14</v>
@@ -1993,15 +1987,15 @@
         <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -2012,7 +2006,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
@@ -2021,12 +2015,12 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
@@ -2035,12 +2029,12 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
@@ -2049,12 +2043,12 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
@@ -2063,12 +2057,12 @@
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
@@ -2081,7 +2075,7 @@
       </c>
     </row>
     <row r="18" spans="2:2">
-      <c r="B18" s="4"/>
+      <c r="B18" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modificate tipologie di test da fare per Requisito
</commit_message>
<xml_diff>
--- a/RP/Esterni/Analisi dei Requisiti/Requisiti.xlsx
+++ b/RP/Esterni/Analisi dei Requisiti/Requisiti.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14700"/>
   </bookViews>
   <sheets>
     <sheet name="Funzionali" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,17 @@
     <sheet name="Vincolo" sheetId="4" r:id="rId4"/>
     <sheet name="Formato Tabelle" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="155">
   <si>
     <t>Codice</t>
   </si>
@@ -179,9 +184,6 @@
     <t>Un \uline{Utente} che ha smarrito la propria password per accedere al sistema potrà modificarla</t>
   </si>
   <si>
-    <t>Un \uline{Utente} che ha smarrito la password ed ha eseguito la procedura di modifica, ne riceverà nella casella di posta, una nuova auto generata randomicamente che dovrà modificare al primo login</t>
-  </si>
-  <si>
     <t xml:space="preserve">RFOB </t>
   </si>
   <si>
@@ -474,13 +476,25 @@
   </si>
   <si>
     <t>Tutte le azioni di tutti gli \uline{utilizzatori}, nel tempo, dovranno essere registrate nel sistema</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>RFOB .1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un \uline{Utente} che ha smarrito la password ed ha eseguito la procedura di modifica, ne riceverà nella casella di posta, una nuova auto generata randomicamente </t>
+  </si>
+  <si>
+    <t>Al primo login la password dovrà essere modificata</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -534,7 +548,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -830,22 +844,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D91"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:D43"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="136" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="5" t="s">
         <v>44</v>
       </c>
@@ -853,9 +867,9 @@
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>33</v>
@@ -864,12 +878,15 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>32</v>
@@ -878,10 +895,13 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="5" t="s">
         <v>43</v>
       </c>
@@ -889,12 +909,12 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -903,62 +923,65 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>53</v>
+        <v>153</v>
       </c>
       <c r="C8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="5" t="s">
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="4" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>30</v>
@@ -967,26 +990,26 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
+    <row r="13" spans="1:5">
+      <c r="A13" s="4" t="s">
         <v>54</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>88</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>36</v>
+        <v>83</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
@@ -995,12 +1018,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>54</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>85</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
@@ -1009,12 +1032,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
@@ -1023,110 +1046,131 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C17" t="s">
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="30">
+        <v>50</v>
+      </c>
+      <c r="E17" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C18" t="s">
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>50</v>
+      </c>
+      <c r="E18" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" t="s">
         <v>25</v>
       </c>
-      <c r="D19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C20" t="s">
-        <v>10</v>
-      </c>
       <c r="D20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="30">
+        <v>50</v>
+      </c>
+      <c r="E20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>108</v>
+        <v>57</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C21" t="s">
         <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>50</v>
+      </c>
+      <c r="E21" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C22" t="s">
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>50</v>
+      </c>
+      <c r="E22" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>110</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="C23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+        <v>50</v>
+      </c>
+      <c r="E23" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="C24" t="s">
         <v>11</v>
@@ -1135,12 +1179,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C25" t="s">
         <v>11</v>
@@ -1149,12 +1193,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="C26" t="s">
         <v>11</v>
@@ -1163,77 +1207,80 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C29" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="28">
+      <c r="A30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C30" t="s">
         <v>96</v>
       </c>
-      <c r="D27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" t="s">
-        <v>54</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" t="s">
         <v>96</v>
       </c>
-      <c r="D28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="30">
-      <c r="A29" t="s">
-        <v>54</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C29" t="s">
-        <v>97</v>
-      </c>
-      <c r="D29" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C30" t="s">
-        <v>97</v>
-      </c>
-      <c r="D30" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="30">
-      <c r="A31" t="s">
-        <v>55</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C31" t="s">
-        <v>99</v>
-      </c>
       <c r="D31" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:5" ht="28">
       <c r="A32" t="s">
         <v>54</v>
       </c>
@@ -1241,163 +1288,172 @@
         <v>101</v>
       </c>
       <c r="C32" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="30">
-      <c r="A33" t="s">
-        <v>55</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="C33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D33" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="28">
       <c r="A34" t="s">
         <v>54</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C34" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D34" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="30">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>104</v>
       </c>
       <c r="C35" t="s">
-        <v>129</v>
+        <v>105</v>
       </c>
       <c r="D35" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" t="s">
+        <v>128</v>
+      </c>
+      <c r="D36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" t="s">
+        <v>128</v>
+      </c>
+      <c r="D37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
         <v>58</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36" t="s">
-        <v>129</v>
-      </c>
-      <c r="D36" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" t="s">
-        <v>59</v>
-      </c>
-      <c r="B37" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C37" t="s">
-        <v>129</v>
-      </c>
-      <c r="D37" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="5" t="s">
+      <c r="C38" t="s">
+        <v>128</v>
+      </c>
+      <c r="D38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B41" s="1" t="s">
+      <c r="D41" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C42" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" t="s">
-        <v>54</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C42" t="s">
-        <v>129</v>
-      </c>
-      <c r="D42" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="D42" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>121</v>
       </c>
       <c r="C43" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D43" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>54</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C44" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D44" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
+        <v>50</v>
+      </c>
+      <c r="E44" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>118</v>
@@ -1409,132 +1465,141 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>34</v>
+        <v>117</v>
       </c>
       <c r="C46" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D46" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>54</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>116</v>
+        <v>34</v>
       </c>
       <c r="C47" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D47" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
+        <v>50</v>
+      </c>
+      <c r="E47" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C48" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D48" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>54</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C49" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D49" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
+        <v>50</v>
+      </c>
+      <c r="E49" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C50" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D50" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C51" t="s">
+        <v>127</v>
+      </c>
+      <c r="D51" t="s">
+        <v>50</v>
+      </c>
+      <c r="E51" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>81</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C52" t="s">
         <v>112</v>
       </c>
-      <c r="C51" t="s">
-        <v>113</v>
-      </c>
-      <c r="D51" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="5" t="s">
+      <c r="D52" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C55" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D54" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" t="s">
-        <v>54</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C55" t="s">
-        <v>39</v>
-      </c>
-      <c r="D55" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="30">
+      <c r="D55" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C56" t="s">
         <v>39</v>
@@ -1543,118 +1608,127 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:5" ht="28">
       <c r="A57" t="s">
         <v>54</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C57" t="s">
+        <v>39</v>
+      </c>
+      <c r="D57" t="s">
+        <v>50</v>
+      </c>
+      <c r="E57" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>53</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C58" t="s">
         <v>42</v>
       </c>
-      <c r="D57" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" t="s">
-        <v>55</v>
-      </c>
-      <c r="B58" s="1" t="s">
+      <c r="D58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>54</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C59" t="s">
+        <v>136</v>
+      </c>
+      <c r="D59" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>56</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C60" t="s">
         <v>137</v>
       </c>
-      <c r="D58" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" t="s">
-        <v>57</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C59" t="s">
-        <v>138</v>
-      </c>
-      <c r="D59" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" t="s">
-        <v>54</v>
-      </c>
-      <c r="B60" s="1" t="s">
+      <c r="D60" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>53</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C60" t="s">
-        <v>132</v>
-      </c>
-      <c r="D60" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="5" t="s">
+      <c r="C61" t="s">
+        <v>131</v>
+      </c>
+      <c r="D61" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B62" s="5"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" t="s">
-        <v>54</v>
-      </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>53</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C64" t="s">
+        <v>31</v>
+      </c>
+      <c r="D64" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>53</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C63" t="s">
-        <v>31</v>
-      </c>
-      <c r="D63" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" t="s">
-        <v>54</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C64" t="s">
+      <c r="C65" t="s">
         <v>28</v>
       </c>
-      <c r="D64" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="A65" t="s">
-        <v>54</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C65" t="s">
-        <v>11</v>
-      </c>
       <c r="D65" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="66" spans="1:4">
+      <c r="E65" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
       <c r="A66" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C66" t="s">
         <v>11</v>
@@ -1663,12 +1737,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="30">
+    <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C67" t="s">
         <v>11</v>
@@ -1677,37 +1751,110 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="2:2">
-      <c r="B91" s="2"/>
+    <row r="68" spans="1:5">
+      <c r="A68" t="s">
+        <v>75</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C68" t="s">
+        <v>11</v>
+      </c>
+      <c r="D68" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2">
+      <c r="B92" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="A63:D63"/>
     <mergeCell ref="A5:D5"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A54:D54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="101.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="101.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="119" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="146.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1715,10 +1862,10 @@
         <v>60</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
         <v>50</v>
@@ -1726,259 +1873,215 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
         <v>60</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="s">
         <v>139</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" t="s">
+        <v>140</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="146.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" t="s">
-        <v>149</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8" t="s">
-        <v>144</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B9" t="s">
-        <v>145</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" t="s">
-        <v>140</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>69</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>69</v>
-      </c>
-      <c r="B12" t="s">
-        <v>142</v>
-      </c>
-      <c r="C12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>70</v>
-      </c>
-      <c r="B13" t="s">
-        <v>141</v>
-      </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>71</v>
-      </c>
-      <c r="B14" t="s">
-        <v>143</v>
-      </c>
-      <c r="C14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="137.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="162.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="112.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="162.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B1" t="s">
         <v>14</v>
@@ -1990,9 +2093,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
         <v>51</v>
@@ -2004,9 +2107,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
@@ -2018,9 +2121,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
@@ -2032,9 +2135,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
@@ -2046,9 +2149,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
@@ -2060,9 +2163,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
@@ -2071,7 +2174,10 @@
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>50</v>
+      </c>
+      <c r="E7" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="2:2">
@@ -2079,25 +2185,29 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2136,5 +2246,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Aggiunti nuovi requisiti derivati dall'incontro del 26/01/2012
</commit_message>
<xml_diff>
--- a/RP/Esterni/Analisi dei Requisiti/Requisiti.xlsx
+++ b/RP/Esterni/Analisi dei Requisiti/Requisiti.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Funzionali" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="162">
   <si>
     <t>Codice</t>
   </si>
@@ -130,9 +130,6 @@
     <t>I campi che potranno essere modificati sono: nome, cognome, indirizzo email, impiego, codice fiscale</t>
   </si>
   <si>
-    <t>Un \uline{Amministratore Sicurezza} dovrà poter modificare l'insieme delle domande di un'azienda</t>
-  </si>
-  <si>
     <t>Una proposta di domanda dovrà essere completamente non \uline{invadente}</t>
   </si>
   <si>
@@ -394,9 +391,6 @@
     <t>I dati personali visualizzabili sono: nome, cognome, codice fiscale, indirizzo di posta elettronica, impiego, password, username</t>
   </si>
   <si>
-    <t>Le statistiche personali sono: punti, trofei, badge</t>
-  </si>
-  <si>
     <t>L'\uline{Amministratore Azienda Autenticato} dovrà poter gestire gli account dei \uline{Dipendenti}</t>
   </si>
   <si>
@@ -427,12 +421,6 @@
     <t>La consultazione farà vedere: il tipo, il testo, le risposte possibili, le risposte corrette, le immagini / video (se presenti), la categoria a cui verrà somministrata, la piattaforma, la temporizzazione (se presente) e il punteggio della domanda</t>
   </si>
   <si>
-    <t>Un \uline{Amministratore Sicurezza} avrà la possibilità di aggiungere una domanda, dall'insieme di quelle già presenti nel database generale</t>
-  </si>
-  <si>
-    <t>Un \uline{Amministratore Sicurezza} avrà la possibilità di rimuovere una domanda dal database di domande da somministrare all'azienda</t>
-  </si>
-  <si>
     <t>UCASA 3.1</t>
   </si>
   <si>
@@ -488,13 +476,46 @@
   </si>
   <si>
     <t>Al primo login la password dovrà essere modificata</t>
+  </si>
+  <si>
+    <t>Un \uline{Dipendente Autenticato} potrà richiedere un numero limitato di domande secondo il tempo trascorso</t>
+  </si>
+  <si>
+    <t>Verbale 26/01/2012</t>
+  </si>
+  <si>
+    <t>RFD</t>
+  </si>
+  <si>
+    <t>Le statistiche personali sono: punti, trofei/badge</t>
+  </si>
+  <si>
+    <t>Un \uline{Amministratore Sicurezza Autenticato} dovrà poter modificare l'insieme delle domande di un'azienda</t>
+  </si>
+  <si>
+    <t>Un \uline{Amministratore Sicurezza Autenticato} avrà la possibilità di aggiungere una domanda, dall'insieme di quelle già presenti nel database generale</t>
+  </si>
+  <si>
+    <t>Un \uline{Amministratore Sicurezza Autenticato} avrà la possibilità di rimuovere una domanda dal database di domande da somministrare all'azienda</t>
+  </si>
+  <si>
+    <t>Il sistema assegnerà in automatico badge/trofei al \uline{Dipendente}, quando questo raggiunge determinati obiettivi di \uline{Gamification}</t>
+  </si>
+  <si>
+    <t>L'\uline{Amministratore Sicurezza Autenticato} dovrà poter modificare i badge o trofei assegnabili agli utenti al raggiungimento di obiettivi di \uline{Gamification}</t>
+  </si>
+  <si>
+    <t>RFOP .1</t>
+  </si>
+  <si>
+    <t>L'\uline{Amministratore Sicurezza Autenticato} dovrà poter modificare gli obiettivi di \uline{Gamification}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -506,6 +527,22 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -528,8 +565,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -547,7 +596,19 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="13">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -845,10 +906,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E92"/>
+  <dimension ref="A1:E96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView topLeftCell="A65" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -861,7 +922,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -869,7 +930,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>33</v>
@@ -881,12 +942,12 @@
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>32</v>
@@ -898,40 +959,43 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
+      <c r="A6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>52</v>
+        <v>146</v>
       </c>
       <c r="C7" t="s">
-        <v>94</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -939,13 +1003,13 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>153</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -953,49 +1017,49 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>152</v>
+        <v>53</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
       </c>
-      <c r="E9" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>148</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="A12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="4" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>30</v>
@@ -1005,25 +1069,25 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" t="s">
+      <c r="A14" s="4" t="s">
         <v>53</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
@@ -1037,7 +1101,7 @@
         <v>53</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
@@ -1048,19 +1112,16 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C17" t="s">
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" t="s">
-        <v>151</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1068,137 +1129,143 @@
         <v>53</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>86</v>
+        <v>151</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>152</v>
       </c>
       <c r="D18" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="E18" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C19" t="s">
         <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E19" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="C21" t="s">
         <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E21" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>107</v>
+        <v>54</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="C22" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E22" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>110</v>
+        <v>56</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C23" t="s">
         <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E23" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>106</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="C24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>9</v>
+        <v>49</v>
+      </c>
+      <c r="E24" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>9</v>
+        <v>49</v>
+      </c>
+      <c r="E25" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="C26" t="s">
         <v>11</v>
@@ -1209,10 +1276,10 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="C27" t="s">
         <v>11</v>
@@ -1226,10 +1293,10 @@
         <v>53</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="C28" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="D28" t="s">
         <v>9</v>
@@ -1237,30 +1304,27 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>122</v>
+        <v>90</v>
       </c>
       <c r="C29" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="D29" t="s">
-        <v>50</v>
-      </c>
-      <c r="E29" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="28">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C30" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D30" t="s">
         <v>9</v>
@@ -1268,100 +1332,103 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="C31" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D31" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+      <c r="E31" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="28">
       <c r="A32" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C32" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D32" t="s">
         <v>9</v>
-      </c>
-      <c r="E32" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C33" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D33" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="28">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C34" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D34" t="s">
-        <v>50</v>
+        <v>9</v>
+      </c>
+      <c r="E34" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" t="s">
+        <v>98</v>
+      </c>
+      <c r="D35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="28">
+      <c r="A36" t="s">
         <v>53</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C35" t="s">
-        <v>105</v>
-      </c>
-      <c r="D35" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" t="s">
-        <v>56</v>
-      </c>
       <c r="B36" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C36" t="s">
-        <v>128</v>
+        <v>98</v>
       </c>
       <c r="D36" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>37</v>
+        <v>103</v>
       </c>
       <c r="C37" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="D37" t="s">
         <v>9</v>
@@ -1369,97 +1436,94 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="C38" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D38" t="s">
         <v>9</v>
       </c>
     </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" t="s">
+        <v>126</v>
+      </c>
+      <c r="D39" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B41" s="1" t="s">
+      <c r="A40" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" t="s">
+        <v>126</v>
+      </c>
+      <c r="D40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" t="s">
-        <v>53</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C43" t="s">
-        <v>128</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="D43" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" t="s">
-        <v>54</v>
+      <c r="A44" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C44" t="s">
-        <v>128</v>
-      </c>
-      <c r="D44" t="s">
-        <v>50</v>
-      </c>
-      <c r="E44" t="s">
-        <v>151</v>
+        <v>122</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C45" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D45" t="s">
         <v>9</v>
@@ -1470,41 +1534,41 @@
         <v>53</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C46" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D46" t="s">
-        <v>9</v>
+        <v>49</v>
+      </c>
+      <c r="E46" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>34</v>
+        <v>117</v>
       </c>
       <c r="C47" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D47" t="s">
-        <v>50</v>
-      </c>
-      <c r="E47" t="s">
-        <v>151</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C48" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D48" t="s">
         <v>9</v>
@@ -1512,30 +1576,30 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>119</v>
+        <v>34</v>
       </c>
       <c r="C49" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D49" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E49" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C50" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D50" t="s">
         <v>9</v>
@@ -1546,122 +1610,125 @@
         <v>53</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C51" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D51" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E51" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C52" t="s">
+        <v>125</v>
+      </c>
+      <c r="D52" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C53" t="s">
+        <v>125</v>
+      </c>
+      <c r="D53" t="s">
+        <v>49</v>
+      </c>
+      <c r="E53" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>80</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" t="s">
         <v>111</v>
       </c>
-      <c r="C52" t="s">
-        <v>112</v>
-      </c>
-      <c r="D52" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C55" s="4" t="s">
+      <c r="D54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C57" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D55" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" t="s">
-        <v>53</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C56" t="s">
-        <v>39</v>
-      </c>
-      <c r="D56" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="28">
-      <c r="A57" t="s">
-        <v>54</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C57" t="s">
-        <v>39</v>
-      </c>
-      <c r="D57" t="s">
-        <v>50</v>
-      </c>
-      <c r="E57" t="s">
-        <v>151</v>
+      <c r="D57" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" t="s">
+        <v>52</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C58" t="s">
+        <v>38</v>
+      </c>
+      <c r="D58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="28">
+      <c r="A59" t="s">
         <v>53</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C58" t="s">
-        <v>42</v>
-      </c>
-      <c r="D58" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" t="s">
-        <v>54</v>
-      </c>
       <c r="B59" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C59" t="s">
-        <v>136</v>
+        <v>38</v>
       </c>
       <c r="D59" t="s">
-        <v>9</v>
+        <v>49</v>
+      </c>
+      <c r="E59" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="C60" t="s">
-        <v>137</v>
+        <v>41</v>
       </c>
       <c r="D60" t="s">
         <v>9</v>
@@ -1672,112 +1739,175 @@
         <v>53</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>40</v>
+        <v>156</v>
       </c>
       <c r="C61" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D61" t="s">
         <v>9</v>
       </c>
     </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>55</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C62" t="s">
+        <v>133</v>
+      </c>
+      <c r="D62" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="63" spans="1:5">
-      <c r="A63" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
+      <c r="A63" t="s">
+        <v>74</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C63" t="s">
+        <v>152</v>
+      </c>
+      <c r="D63" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" t="s">
-        <v>53</v>
+        <v>160</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="C64" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="D64" t="s">
         <v>9</v>
       </c>
       <c r="E64" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>147</v>
+        <v>39</v>
       </c>
       <c r="C65" t="s">
-        <v>28</v>
+        <v>129</v>
       </c>
       <c r="D65" t="s">
         <v>9</v>
       </c>
-      <c r="E65" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
-      <c r="A66" t="s">
-        <v>53</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C66" t="s">
-        <v>11</v>
-      </c>
-      <c r="D66" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="67" spans="1:5">
-      <c r="A67" t="s">
-        <v>53</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C67" t="s">
-        <v>11</v>
-      </c>
-      <c r="D67" t="s">
-        <v>9</v>
-      </c>
+      <c r="A67" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
+        <v>52</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C68" t="s">
+        <v>31</v>
+      </c>
+      <c r="D68" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" t="s">
+        <v>52</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C69" t="s">
+        <v>28</v>
+      </c>
+      <c r="D69" t="s">
+        <v>9</v>
+      </c>
+      <c r="E69" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>52</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C70" t="s">
+        <v>11</v>
+      </c>
+      <c r="D70" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
+        <v>52</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C71" t="s">
+        <v>11</v>
+      </c>
+      <c r="D71" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
+        <v>74</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C68" t="s">
+      <c r="C72" t="s">
         <v>11</v>
       </c>
-      <c r="D68" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="92" spans="2:2">
-      <c r="B92" s="2"/>
+      <c r="D72" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2">
+      <c r="B96" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A63:D63"/>
-    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A67:D67"/>
+    <mergeCell ref="A6:D6"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A56:D56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1804,7 +1934,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
@@ -1816,15 +1946,15 @@
         <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -1847,7 +1977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -1859,7 +1989,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
         <v>22</v>
@@ -1868,12 +1998,12 @@
         <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
         <v>21</v>
@@ -1882,12 +2012,12 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
@@ -1896,54 +2026,54 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
         <v>23</v>
@@ -1952,15 +2082,15 @@
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B8" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -1971,10 +2101,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -1985,21 +2115,21 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B11" t="s">
         <v>24</v>
@@ -2008,49 +2138,49 @@
         <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B14" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -2081,7 +2211,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
         <v>14</v>
@@ -2090,15 +2220,15 @@
         <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -2109,7 +2239,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
@@ -2118,12 +2248,12 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
@@ -2132,12 +2262,12 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
@@ -2146,12 +2276,12 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
@@ -2160,12 +2290,12 @@
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
@@ -2174,10 +2304,10 @@
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="2:2">

</xml_diff>

<commit_message>
piccolo errore di numerazione
</commit_message>
<xml_diff>
--- a/RP/Esterni/Analisi dei Requisiti/Requisiti.xlsx
+++ b/RP/Esterni/Analisi dei Requisiti/Requisiti.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Funzionali" sheetId="1" r:id="rId1"/>
@@ -908,8 +908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1585,7 +1585,7 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>151</v>
@@ -2137,7 +2137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Modifiche minori all'AR e file Excel
</commit_message>
<xml_diff>
--- a/RP/Esterni/Analisi dei Requisiti/Requisiti.xlsx
+++ b/RP/Esterni/Analisi dei Requisiti/Requisiti.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="163">
   <si>
     <t>Codice</t>
   </si>
@@ -487,9 +487,6 @@
     <t>Un \uline{Amministratore Sicurezza Autenticato} avrà la possibilità di aggiungere una domanda, dall'insieme di quelle già presenti nel database generale</t>
   </si>
   <si>
-    <t>Un \uline{Amministratore Sicurezza Autenticato} avrà la possibilità di rimuovere una domanda dal database di domande da somministrare all'azienda</t>
-  </si>
-  <si>
     <t>Il sistema assegnerà in automatico badge/trofei al \uline{Dipendente}, quando questo raggiunge determinati obiettivi di \uline{Gamification}</t>
   </si>
   <si>
@@ -509,13 +506,19 @@
   </si>
   <si>
     <t>Il sistema dovrà essere multipiattaforma (per quanto riguarda i \uline{dispositivi fissi})</t>
+  </si>
+  <si>
+    <t>Statico</t>
+  </si>
+  <si>
+    <t>Un \uline{Amministratore Sicurezza Autenticato} avrà la possibilità di rimuovere una domanda dal database di domande da somministrare all'utente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -597,19 +600,19 @@
     </xf>
   </cellXfs>
   <cellStyles count="13">
-    <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale visitato" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale visitato" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale visitato" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale visitato" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale visitato" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale visitato" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -905,19 +908,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="136" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -939,7 +942,7 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -953,7 +956,7 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -961,13 +964,13 @@
         <v>150</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C4" t="s">
         <v>149</v>
       </c>
       <c r="D4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -989,7 +992,7 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1003,10 +1006,10 @@
         <v>91</v>
       </c>
       <c r="D8" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -1017,7 +1020,7 @@
         <v>91</v>
       </c>
       <c r="D9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1031,7 +1034,7 @@
         <v>91</v>
       </c>
       <c r="D10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1053,7 +1056,7 @@
         <v>29</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1067,7 +1070,7 @@
         <v>29</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1081,7 +1084,7 @@
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1095,7 +1098,7 @@
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1109,7 +1112,7 @@
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1123,7 +1126,7 @@
         <v>149</v>
       </c>
       <c r="D18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1140,7 +1143,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="30">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -1154,7 +1157,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="30">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -1196,7 +1199,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>104</v>
       </c>
@@ -1235,7 +1238,7 @@
         <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1249,7 +1252,7 @@
         <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1263,10 +1266,10 @@
         <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="30">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -1277,7 +1280,7 @@
         <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1291,7 +1294,7 @@
         <v>92</v>
       </c>
       <c r="D30" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1308,7 +1311,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="30">
+    <row r="32" spans="1:4" ht="28">
       <c r="A32" t="s">
         <v>50</v>
       </c>
@@ -1319,7 +1322,7 @@
         <v>93</v>
       </c>
       <c r="D32" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1336,7 +1339,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="30">
+    <row r="34" spans="1:5" ht="28">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -1347,7 +1350,7 @@
         <v>95</v>
       </c>
       <c r="D34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1361,10 +1364,10 @@
         <v>96</v>
       </c>
       <c r="D35" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="30">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="28">
       <c r="A36" t="s">
         <v>51</v>
       </c>
@@ -1389,7 +1392,7 @@
         <v>102</v>
       </c>
       <c r="D37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1411,7 +1414,7 @@
         <v>111</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1425,7 +1428,7 @@
         <v>121</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E41" s="4"/>
     </row>
@@ -1440,7 +1443,7 @@
         <v>124</v>
       </c>
       <c r="D42" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1457,7 +1460,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="30">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>53</v>
       </c>
@@ -1468,7 +1471,7 @@
         <v>124</v>
       </c>
       <c r="D44" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1482,7 +1485,7 @@
         <v>124</v>
       </c>
       <c r="D45" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1496,7 +1499,7 @@
         <v>124</v>
       </c>
       <c r="D46" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1510,7 +1513,7 @@
         <v>126</v>
       </c>
       <c r="D47" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1524,7 +1527,7 @@
         <v>125</v>
       </c>
       <c r="D48" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1552,7 +1555,7 @@
         <v>122</v>
       </c>
       <c r="D50" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1580,7 +1583,7 @@
         <v>123</v>
       </c>
       <c r="D52" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1602,13 +1605,13 @@
         <v>78</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C54" t="s">
         <v>123</v>
       </c>
       <c r="D54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1622,7 +1625,7 @@
         <v>109</v>
       </c>
       <c r="D55" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1644,7 +1647,7 @@
         <v>28</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1658,10 +1661,10 @@
         <v>37</v>
       </c>
       <c r="D59" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="30">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="28">
       <c r="A60" t="s">
         <v>51</v>
       </c>
@@ -1686,10 +1689,10 @@
         <v>40</v>
       </c>
       <c r="D61" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="30">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62" t="s">
         <v>51</v>
       </c>
@@ -1700,21 +1703,21 @@
         <v>130</v>
       </c>
       <c r="D62" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="30">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
       <c r="A63" t="s">
         <v>53</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C63" t="s">
         <v>131</v>
       </c>
       <c r="D63" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1722,27 +1725,27 @@
         <v>72</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C64" t="s">
         <v>149</v>
       </c>
       <c r="D64" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="30">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C65" t="s">
         <v>149</v>
       </c>
       <c r="D65" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1756,7 +1759,7 @@
         <v>127</v>
       </c>
       <c r="D66" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1778,7 +1781,7 @@
         <v>30</v>
       </c>
       <c r="D69" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1792,7 +1795,7 @@
         <v>27</v>
       </c>
       <c r="D70" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1806,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="D71" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1820,10 +1823,10 @@
         <v>10</v>
       </c>
       <c r="D72" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="30">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -1834,7 +1837,7 @@
         <v>10</v>
       </c>
       <c r="D73" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="97" spans="2:2">
@@ -1850,7 +1853,6 @@
     <mergeCell ref="A57:D57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1860,18 +1862,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="101.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="101.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="119" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1886,7 +1888,7 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1900,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -1914,17 +1916,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="146.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="146.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2036,7 +2038,7 @@
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2050,7 +2052,7 @@
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2134,19 +2136,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="112.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="162.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="112.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="162.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2168,13 +2170,13 @@
         <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2261,20 +2263,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">

</xml_diff>

<commit_message>
rimodificato un requisito (RFOB 29.2) utente --> dipendenti (con sottolineatura)
</commit_message>
<xml_diff>
--- a/RP/Esterni/Analisi dei Requisiti/Requisiti.xlsx
+++ b/RP/Esterni/Analisi dei Requisiti/Requisiti.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="162">
   <si>
     <t>Codice</t>
   </si>
@@ -508,17 +508,14 @@
     <t>Il sistema dovrà essere multipiattaforma (per quanto riguarda i \uline{dispositivi fissi})</t>
   </si>
   <si>
-    <t>Statico</t>
-  </si>
-  <si>
-    <t>Un \uline{Amministratore Sicurezza Autenticato} avrà la possibilità di rimuovere una domanda dal database di domande da somministrare all'utente</t>
+    <t>Un \uline{Amministratore Sicurezza Autenticato} avrà la possibilità di rimuovere una domanda dal database di domande da somministrare ai \uline{Dipendenti}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -600,19 +597,19 @@
     </xf>
   </cellXfs>
   <cellStyles count="13">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale visitato" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale visitato" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale visitato" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale visitato" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale visitato" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale visitato" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -908,19 +905,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="136" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="135.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1009,7 +1006,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" ht="30">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -1098,7 +1095,7 @@
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>161</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1143,7 +1140,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" ht="30">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -1157,7 +1154,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" ht="30">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -1199,7 +1196,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" ht="30">
       <c r="A24" t="s">
         <v>104</v>
       </c>
@@ -1269,7 +1266,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" ht="30">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -1311,7 +1308,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="28">
+    <row r="32" spans="1:4" ht="30">
       <c r="A32" t="s">
         <v>50</v>
       </c>
@@ -1339,7 +1336,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="28">
+    <row r="34" spans="1:5" ht="30">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -1367,7 +1364,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="28">
+    <row r="36" spans="1:5" ht="30">
       <c r="A36" t="s">
         <v>51</v>
       </c>
@@ -1460,7 +1457,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" ht="30">
       <c r="A44" t="s">
         <v>53</v>
       </c>
@@ -1664,7 +1661,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="28">
+    <row r="60" spans="1:4" ht="30">
       <c r="A60" t="s">
         <v>51</v>
       </c>
@@ -1692,7 +1689,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" ht="30">
       <c r="A62" t="s">
         <v>51</v>
       </c>
@@ -1706,12 +1703,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" ht="30">
       <c r="A63" t="s">
         <v>53</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C63" t="s">
         <v>131</v>
@@ -1734,7 +1731,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" ht="30">
       <c r="A65" t="s">
         <v>156</v>
       </c>
@@ -1826,7 +1823,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" ht="30">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -1862,19 +1859,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="101.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="119" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="101.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1916,17 +1912,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="146.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.1640625" customWidth="1"/>
+    <col min="2" max="2" width="146.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2136,19 +2132,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="112.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="162.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="112.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="162.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2263,20 +2259,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">

</xml_diff>

<commit_message>
Aggiornato un requisito non tracciato.
</commit_message>
<xml_diff>
--- a/RP/Esterni/Analisi dei Requisiti/Requisiti.xlsx
+++ b/RP/Esterni/Analisi dei Requisiti/Requisiti.xlsx
@@ -334,15 +334,9 @@
     <t>UCDA 8</t>
   </si>
   <si>
-    <t>Il tipo delle risposte può essere: si/no, risposta chiusa, risposta multipla.</t>
-  </si>
-  <si>
     <t>RFD .2.2</t>
   </si>
   <si>
-    <t>Il tipo delle risposte può essere: domanda con video, domanda con foto (entrambe con le modalità sopra citate),  scansione QR nel tempo limite, scansione QR nell'ordine corretto.</t>
-  </si>
-  <si>
     <t>Il tipo delle risposte può essere: ordinamento di frasi o foto, trova errori nella foto, trova differenze nella foto, registra gli RF-ID nell'ordine corretto</t>
   </si>
   <si>
@@ -509,6 +503,12 @@
   </si>
   <si>
     <t>Un \uline{Amministratore Sicurezza Autenticato} avrà la possibilità di rimuovere una domanda dal database di domande da somministrare ai \uline{Dipendenti}</t>
+  </si>
+  <si>
+    <t>Il tipo delle risposte può essere: si/no, risposta chiusa, risposta multipla</t>
+  </si>
+  <si>
+    <t>Il tipo delle risposte può essere: domanda con video, domanda con foto (entrambe con le modalità sopra citate),  scansione QR nel tempo limite, scansione QR nell'ordine corretto</t>
   </si>
 </sst>
 </file>
@@ -908,8 +908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -939,7 +939,7 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -953,21 +953,21 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -983,13 +983,13 @@
         <v>50</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1003,7 +1003,7 @@
         <v>91</v>
       </c>
       <c r="D8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30">
@@ -1011,27 +1011,27 @@
         <v>51</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C9" t="s">
         <v>91</v>
       </c>
       <c r="D9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
+        <v>143</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>147</v>
       </c>
       <c r="C10" t="s">
         <v>91</v>
       </c>
       <c r="D10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1053,7 +1053,7 @@
         <v>29</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1067,7 +1067,7 @@
         <v>29</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1081,7 +1081,7 @@
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1109,7 +1109,7 @@
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1117,13 +1117,13 @@
         <v>51</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1187,7 +1187,7 @@
         <v>54</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>103</v>
+        <v>160</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
@@ -1198,10 +1198,10 @@
     </row>
     <row r="24" spans="1:4" ht="30">
       <c r="A24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>105</v>
+        <v>161</v>
       </c>
       <c r="C24" t="s">
         <v>9</v>
@@ -1212,10 +1212,10 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C25" t="s">
         <v>9</v>
@@ -1235,7 +1235,7 @@
         <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1249,7 +1249,7 @@
         <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1263,7 +1263,7 @@
         <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30">
@@ -1277,7 +1277,7 @@
         <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1291,7 +1291,7 @@
         <v>92</v>
       </c>
       <c r="D30" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1299,7 +1299,7 @@
         <v>50</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C31" t="s">
         <v>92</v>
@@ -1319,7 +1319,7 @@
         <v>93</v>
       </c>
       <c r="D32" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1347,7 +1347,7 @@
         <v>95</v>
       </c>
       <c r="D34" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1361,7 +1361,7 @@
         <v>96</v>
       </c>
       <c r="D35" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="30">
@@ -1389,7 +1389,7 @@
         <v>102</v>
       </c>
       <c r="D37" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1405,13 +1405,13 @@
         <v>78</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1419,13 +1419,13 @@
         <v>78</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E41" s="4"/>
     </row>
@@ -1434,13 +1434,13 @@
         <v>50</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C42" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D42" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1448,10 +1448,10 @@
         <v>51</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C43" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D43" t="s">
         <v>48</v>
@@ -1465,10 +1465,10 @@
         <v>100</v>
       </c>
       <c r="C44" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D44" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1479,10 +1479,10 @@
         <v>35</v>
       </c>
       <c r="C45" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D45" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1493,10 +1493,10 @@
         <v>36</v>
       </c>
       <c r="C46" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D46" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1504,13 +1504,13 @@
         <v>50</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C47" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D47" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1518,13 +1518,13 @@
         <v>50</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C48" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D48" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1535,7 +1535,7 @@
         <v>33</v>
       </c>
       <c r="C49" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D49" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
         <v>50</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C50" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D50" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1560,10 +1560,10 @@
         <v>51</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C51" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D51" t="s">
         <v>48</v>
@@ -1574,13 +1574,13 @@
         <v>50</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C52" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D52" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1588,10 +1588,10 @@
         <v>51</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C53" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D53" t="s">
         <v>48</v>
@@ -1602,13 +1602,13 @@
         <v>78</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C54" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D54" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1616,13 +1616,13 @@
         <v>78</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C55" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D55" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1644,7 +1644,7 @@
         <v>28</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1652,13 +1652,13 @@
         <v>50</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C59" t="s">
         <v>37</v>
       </c>
       <c r="D59" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="30">
@@ -1666,7 +1666,7 @@
         <v>51</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C60" t="s">
         <v>37</v>
@@ -1680,13 +1680,13 @@
         <v>50</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C61" t="s">
         <v>40</v>
       </c>
       <c r="D61" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="30">
@@ -1694,13 +1694,13 @@
         <v>51</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C62" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D62" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="30">
@@ -1708,13 +1708,13 @@
         <v>53</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C63" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D63" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1722,27 +1722,27 @@
         <v>72</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C64" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D64" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="30">
       <c r="A65" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C65" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D65" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1753,10 +1753,10 @@
         <v>38</v>
       </c>
       <c r="C66" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D66" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1772,13 +1772,13 @@
         <v>50</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C69" t="s">
         <v>30</v>
       </c>
       <c r="D69" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1786,13 +1786,13 @@
         <v>50</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C70" t="s">
         <v>27</v>
       </c>
       <c r="D70" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1806,7 +1806,7 @@
         <v>10</v>
       </c>
       <c r="D71" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1820,7 +1820,7 @@
         <v>10</v>
       </c>
       <c r="D72" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="30">
@@ -1834,7 +1834,7 @@
         <v>10</v>
       </c>
       <c r="D73" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="97" spans="2:2">
@@ -1884,7 +1884,7 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1892,13 +1892,13 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -1972,7 +1972,7 @@
         <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -1986,7 +1986,7 @@
         <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -2028,13 +2028,13 @@
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2042,13 +2042,13 @@
         <v>64</v>
       </c>
       <c r="B9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2056,7 +2056,7 @@
         <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
@@ -2084,7 +2084,7 @@
         <v>65</v>
       </c>
       <c r="B12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
@@ -2098,7 +2098,7 @@
         <v>66</v>
       </c>
       <c r="B13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
@@ -2112,7 +2112,7 @@
         <v>67</v>
       </c>
       <c r="B14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
@@ -2166,13 +2166,13 @@
         <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2233,7 +2233,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
AR: fix altezza righe xlsx requisiti
</commit_message>
<xml_diff>
--- a/RP/Esterni/Analisi dei Requisiti/Requisiti.xlsx
+++ b/RP/Esterni/Analisi dei Requisiti/Requisiti.xlsx
@@ -909,13 +909,13 @@
   <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="135.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="148.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1006,7 +1006,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30">
+    <row r="9" spans="1:4" ht="15" customHeight="1">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -1034,6 +1034,9 @@
         <v>157</v>
       </c>
     </row>
+    <row r="11" spans="1:4">
+      <c r="B11" s="2"/>
+    </row>
     <row r="12" spans="1:4">
       <c r="A12" s="5" t="s">
         <v>43</v>
@@ -1140,7 +1143,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="30">
+    <row r="20" spans="1:4" ht="15" customHeight="1">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -1154,7 +1157,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="30">
+    <row r="21" spans="1:4" ht="15.75" customHeight="1">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -1266,7 +1269,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="30">
+    <row r="29" spans="1:4" ht="15" customHeight="1">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -1457,7 +1460,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="30">
+    <row r="44" spans="1:5" ht="15" customHeight="1">
       <c r="A44" t="s">
         <v>53</v>
       </c>
@@ -1689,7 +1692,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="30">
+    <row r="62" spans="1:4" ht="15" customHeight="1">
       <c r="A62" t="s">
         <v>51</v>
       </c>
@@ -1703,7 +1706,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="30">
+    <row r="63" spans="1:4" ht="15" customHeight="1">
       <c r="A63" t="s">
         <v>53</v>
       </c>
@@ -1731,7 +1734,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="30">
+    <row r="65" spans="1:4" ht="15" customHeight="1">
       <c r="A65" t="s">
         <v>154</v>
       </c>
@@ -1823,7 +1826,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="30">
+    <row r="73" spans="1:4" ht="15" customHeight="1">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -1850,6 +1853,7 @@
     <mergeCell ref="A57:D57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
mancava un .1 su una cella
</commit_message>
<xml_diff>
--- a/RP/Esterni/Analisi dei Requisiti/Requisiti.xlsx
+++ b/RP/Esterni/Analisi dei Requisiti/Requisiti.xlsx
@@ -908,8 +908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1299,7 +1299,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>117</v>

</xml_diff>